<commit_message>
Single and Multi Isothemal Translation OK
</commit_message>
<xml_diff>
--- a/output_NaCl_MI.xlsx
+++ b/output_NaCl_MI.xlsx
@@ -636,7 +636,7 @@
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>Temperaturas isotermas</t>
+          <t>Isothermal Temperatures</t>
         </is>
       </c>
       <c r="AP1" s="1" t="n">
@@ -684,22 +684,22 @@
         <v>293.15</v>
       </c>
       <c r="E2" t="n">
-        <v>0.276178096374457</v>
+        <v>0.2761774875984328</v>
       </c>
       <c r="F2" t="n">
-        <v>-11.31672781099762</v>
+        <v>-11.3167272320194</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9939144607055734</v>
+        <v>0.9939144607055735</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9869437986972225</v>
+        <v>0.9869437986972197</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.002731136492815964</v>
+        <v>0.002731137146338852</v>
       </c>
       <c r="K2" t="n">
         <v>-0</v>
@@ -708,25 +708,25 @@
         <v>293.15</v>
       </c>
       <c r="M2" t="n">
-        <v>-4.119732820159863</v>
+        <v>-4.119732656159664</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9996950177053986</v>
+        <v>0.9996950176947542</v>
       </c>
       <c r="O2" t="n">
-        <v>0.006341955711380692</v>
+        <v>0.006341955936972853</v>
       </c>
       <c r="P2" t="n">
-        <v>0.02278607388206988</v>
+        <v>0.02278607188089687</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.1840919037094783</v>
+        <v>0.1840919041015912</v>
       </c>
       <c r="R2" t="n">
         <v>1</v>
       </c>
       <c r="S2" t="n">
-        <v>5.014323837140823</v>
+        <v>5.01432383171402</v>
       </c>
       <c r="T2" t="n">
         <v>0.2572289559331421</v>
@@ -747,43 +747,43 @@
         <v>6.137529767019371</v>
       </c>
       <c r="Z2" t="n">
-        <v>6.128248033043786</v>
+        <v>6.128248030823316</v>
       </c>
       <c r="AA2" t="n">
         <v>0.9882078962987058</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.9870052875588482</v>
+        <v>0.9870052872714427</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.9999062071212282</v>
+        <v>0.9999062071147516</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.01455655867742182</v>
+        <v>0.0145565594366513</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.0403747113392452</v>
+        <v>0.04037471203000731</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.00515119116610055</v>
+        <v>0.005151191322087243</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.02419816420803144</v>
+        <v>0.02419816211833436</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.9999759695841097</v>
+        <v>0.9999759695833863</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.001259088019427938</v>
+        <v>0.001259088071394117</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.005439748642629416</v>
+        <v>0.00543974873554065</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.001331658121112442</v>
+        <v>0.001331658188963548</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.005037661609325461</v>
+        <v>0.005037661695335184</v>
       </c>
       <c r="AM2" t="n">
         <v>0</v>
@@ -795,34 +795,34 @@
         <v>293.15</v>
       </c>
       <c r="AP2" t="n">
-        <v>6.128248033043786</v>
+        <v>6.128248030823316</v>
       </c>
       <c r="AQ2" t="n">
-        <v>6.297792037214233</v>
+        <v>6.297792041754176</v>
       </c>
       <c r="AR2" t="n">
-        <v>6.493884278168232</v>
+        <v>6.493884284656833</v>
       </c>
       <c r="AS2" t="n">
-        <v>6.589328014701029</v>
+        <v>6.589328019813424</v>
       </c>
       <c r="AT2" t="n">
-        <v>6.714214586332216</v>
+        <v>6.714214587311663</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.9870052875588484</v>
+        <v>0.9870052872714429</v>
       </c>
       <c r="AV2" t="n">
-        <v>1.105048531458197</v>
+        <v>1.105048532107958</v>
       </c>
       <c r="AW2" t="n">
-        <v>1.246982030915557</v>
+        <v>1.246982031921</v>
       </c>
       <c r="AX2" t="n">
-        <v>1.315193816278754</v>
+        <v>1.315193817087749</v>
       </c>
       <c r="AY2" t="n">
-        <v>1.398255996140206</v>
+        <v>1.398255996295874</v>
       </c>
     </row>
     <row r="3">
@@ -839,10 +839,10 @@
         <v>318.15</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0002479380263591208</v>
+        <v>0.0002479376566248699</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.008292670340228191</v>
+        <v>-0.008292670042961626</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -850,16 +850,16 @@
         <v>0.01498387603282741</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.08448671876932588</v>
+        <v>-0.0844867181158919</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.08155409957224864</v>
+        <v>-0.08155409947948911</v>
       </c>
       <c r="L3" t="n">
         <v>293.15</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.005116164857689253</v>
+        <v>-0.005116165391258863</v>
       </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
@@ -867,10 +867,10 @@
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
-        <v>5.014323837139557</v>
+        <v>5.014323831714025</v>
       </c>
       <c r="T3" t="n">
-        <v>0.2576846789182338</v>
+        <v>0.2576846789180672</v>
       </c>
       <c r="U3" t="n">
         <v>293.15</v>
@@ -888,13 +888,13 @@
         <v>5.782927553365466</v>
       </c>
       <c r="Z3" t="n">
-        <v>5.792714619537015</v>
+        <v>5.792714617666035</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.9407441685492667</v>
+        <v>0.9407441685491847</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.9419130312900763</v>
+        <v>0.9419130310662983</v>
       </c>
       <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr"/>
@@ -916,34 +916,34 @@
         <v>318.15</v>
       </c>
       <c r="AP3" t="n">
-        <v>5.414401840148177</v>
+        <v>5.414401838517713</v>
       </c>
       <c r="AQ3" t="n">
-        <v>5.578523355101138</v>
+        <v>5.578523358685096</v>
       </c>
       <c r="AR3" t="n">
-        <v>5.758637392549446</v>
+        <v>5.758637396361909</v>
       </c>
       <c r="AS3" t="n">
-        <v>5.842417190856072</v>
+        <v>5.842417192551233</v>
       </c>
       <c r="AT3" t="n">
-        <v>5.947922618188086</v>
+        <v>5.947922614965097</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.8944102322049637</v>
+        <v>0.8944102320270182</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.9977652440956526</v>
+        <v>0.9977652445421379</v>
       </c>
       <c r="AW3" t="n">
-        <v>1.122455499753153</v>
+        <v>1.122455500290107</v>
       </c>
       <c r="AX3" t="n">
-        <v>1.182587435420557</v>
+        <v>1.182587435671948</v>
       </c>
       <c r="AY3" t="n">
-        <v>1.256081657606512</v>
+        <v>1.256081657120436</v>
       </c>
     </row>
     <row r="4">
@@ -960,10 +960,10 @@
         <v>348.15</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2577238355558587</v>
+        <v>0.2577239617380637</v>
       </c>
       <c r="F4" t="n">
-        <v>2.455071226777757</v>
+        <v>2.455071109815996</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
@@ -971,16 +971,16 @@
         <v>0.0312420334115468</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.1603117299433889</v>
+        <v>-0.1603117292901621</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.1642708357151875</v>
+        <v>-0.1642708355659348</v>
       </c>
       <c r="L4" t="n">
         <v>293.15</v>
       </c>
       <c r="M4" t="n">
-        <v>13.90575324956906</v>
+        <v>13.90575250931942</v>
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
@@ -988,10 +988,10 @@
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="n">
-        <v>5.014323837139642</v>
+        <v>5.01432383171399</v>
       </c>
       <c r="T4" t="n">
-        <v>0.2587619336602568</v>
+        <v>0.258761933659696</v>
       </c>
       <c r="U4" t="n">
         <v>293.15</v>
@@ -1009,13 +1009,13 @@
         <v>5.468736985077713</v>
       </c>
       <c r="Z4" t="n">
-        <v>5.455780147792999</v>
+        <v>5.455780146144386</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.9008713445422822</v>
+        <v>0.9008713445420172</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.8994427502198568</v>
+        <v>0.899442750038091</v>
       </c>
       <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="inlineStr"/>
@@ -1037,34 +1037,34 @@
         <v>348.15</v>
       </c>
       <c r="AP4" t="n">
-        <v>4.811022213183165</v>
+        <v>4.811022211572012</v>
       </c>
       <c r="AQ4" t="n">
-        <v>4.973268191742228</v>
+        <v>4.973268194330408</v>
       </c>
       <c r="AR4" t="n">
-        <v>5.144519410203</v>
+        <v>5.144519412036297</v>
       </c>
       <c r="AS4" t="n">
-        <v>5.221558622960295</v>
+        <v>5.221558622327353</v>
       </c>
       <c r="AT4" t="n">
-        <v>5.315959776368129</v>
+        <v>5.315959770544107</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.8252066555423917</v>
+        <v>0.8252066553917152</v>
       </c>
       <c r="AV4" t="n">
-        <v>0.9156790601704112</v>
+        <v>0.915679060454511</v>
       </c>
       <c r="AW4" t="n">
-        <v>1.024758622173074</v>
+        <v>1.024758622411511</v>
       </c>
       <c r="AX4" t="n">
-        <v>1.077260921313165</v>
+        <v>1.077260921234938</v>
       </c>
       <c r="AY4" t="n">
-        <v>1.141210227681547</v>
+        <v>1.141210226855637</v>
       </c>
     </row>
     <row r="5">
@@ -1088,16 +1088,16 @@
         <v>0.04879697963973732</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.2523805625668641</v>
+        <v>-0.2523805619139925</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.2472266612189586</v>
+        <v>-0.2472266610548279</v>
       </c>
       <c r="L5" t="n">
         <v>293.15</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.02565108472344577</v>
+        <v>-0.02565108249981839</v>
       </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
@@ -1105,10 +1105,10 @@
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="n">
-        <v>5.014323837139757</v>
+        <v>5.014323831714001</v>
       </c>
       <c r="T5" t="n">
-        <v>0.2606029123198563</v>
+        <v>0.2606029123186184</v>
       </c>
       <c r="U5" t="n">
         <v>293.15</v>
@@ -1126,13 +1126,13 @@
         <v>5.105214675543413</v>
       </c>
       <c r="Z5" t="n">
-        <v>5.121681614974557</v>
+        <v>5.121681613412028</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.8582286410176487</v>
+        <v>0.8582286410170904</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.8598896715108781</v>
+        <v>0.8598896713523952</v>
       </c>
       <c r="AC5" t="inlineStr"/>
       <c r="AD5" t="inlineStr"/>
@@ -1154,34 +1154,34 @@
         <v>363.15</v>
       </c>
       <c r="AP5" t="n">
-        <v>4.302963958847759</v>
+        <v>4.302963956871606</v>
       </c>
       <c r="AQ5" t="n">
-        <v>4.463712345881199</v>
+        <v>4.463712347492084</v>
       </c>
       <c r="AR5" t="n">
-        <v>4.628479852346993</v>
+        <v>4.628479852743525</v>
       </c>
       <c r="AS5" t="n">
-        <v>4.700750718555739</v>
+        <v>4.700750716386049</v>
       </c>
       <c r="AT5" t="n">
-        <v>4.787528768458696</v>
+        <v>4.787528761129073</v>
       </c>
       <c r="AU5" t="n">
-        <v>0.7723474090186396</v>
+        <v>0.7723474088587626</v>
       </c>
       <c r="AV5" t="n">
-        <v>0.8516169111344973</v>
+        <v>0.8516169112924314</v>
       </c>
       <c r="AW5" t="n">
-        <v>0.9468988599460897</v>
+        <v>0.9468988600008414</v>
       </c>
       <c r="AX5" t="n">
-        <v>0.9925155367538016</v>
+        <v>0.9925155364965056</v>
       </c>
       <c r="AY5" t="n">
-        <v>1.04763147860313</v>
+        <v>1.047631477635831</v>
       </c>
     </row>
     <row r="6">
@@ -1201,16 +1201,16 @@
         <v>0.06765257034703157</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.3346791797636436</v>
+        <v>-0.3346791791113101</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.3294396100586554</v>
+        <v>-0.3294396099253206</v>
       </c>
       <c r="L6" t="n">
         <v>293.15</v>
       </c>
       <c r="M6" t="n">
-        <v>-9.288089472603748</v>
+        <v>-9.288088717062575</v>
       </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
@@ -1218,10 +1218,10 @@
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="n">
-        <v>5.014323837139873</v>
+        <v>5.014323831714021</v>
       </c>
       <c r="T6" t="n">
-        <v>0.2633660036526261</v>
+        <v>0.2633660036503637</v>
       </c>
       <c r="U6" t="n">
         <v>293.15</v>
@@ -1239,13 +1239,13 @@
         <v>4.778384826733895</v>
       </c>
       <c r="Z6" t="n">
-        <v>4.79470049348119</v>
+        <v>4.794700491863904</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.8219305475800203</v>
+        <v>0.8219305475790414</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.82343676610655</v>
+        <v>0.8234367659559623</v>
       </c>
       <c r="AC6" t="inlineStr"/>
       <c r="AD6" t="inlineStr"/>
@@ -1267,34 +1267,34 @@
         <v>383.15</v>
       </c>
       <c r="AP6" t="n">
-        <v>3.875870960726973</v>
+        <v>3.875870958156469</v>
       </c>
       <c r="AQ6" t="n">
-        <v>4.033989700482301</v>
+        <v>4.033989701185501</v>
       </c>
       <c r="AR6" t="n">
-        <v>4.192349772994856</v>
+        <v>4.192349772375101</v>
       </c>
       <c r="AS6" t="n">
-        <v>4.260409039292942</v>
+        <v>4.260409036169515</v>
       </c>
       <c r="AT6" t="n">
-        <v>4.340811746008054</v>
+        <v>4.340811737940812</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.7310457624753597</v>
+        <v>0.7310457622947394</v>
       </c>
       <c r="AV6" t="n">
-        <v>0.8006353818955247</v>
+        <v>0.8006353819594491</v>
       </c>
       <c r="AW6" t="n">
-        <v>0.8838908036882899</v>
+        <v>0.8838908036365465</v>
       </c>
       <c r="AX6" t="n">
-        <v>0.9234378308193709</v>
+        <v>0.9234378304810216</v>
       </c>
       <c r="AY6" t="n">
-        <v>0.9706642843055285</v>
+        <v>0.9706642833221828</v>
       </c>
     </row>
     <row r="7">
@@ -1310,16 +1310,16 @@
         <v>0.110582991288982</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.4983814409367217</v>
+        <v>-0.498381440286268</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.4925579748075635</v>
+        <v>-0.4925579748890826</v>
       </c>
       <c r="L7" t="n">
         <v>293.15</v>
       </c>
       <c r="M7" t="n">
-        <v>0.005279786998163992</v>
+        <v>0.005279784800695957</v>
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -1327,10 +1327,10 @@
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="n">
-        <v>5.014323837139864</v>
+        <v>5.014323831714044</v>
       </c>
       <c r="T7" t="n">
-        <v>0.2727492686425728</v>
+        <v>0.2727492686367511</v>
       </c>
       <c r="U7" t="n">
         <v>293.15</v>
@@ -1348,13 +1348,13 @@
         <v>4.142185188607134</v>
       </c>
       <c r="Z7" t="n">
-        <v>4.159245007531394</v>
+        <v>4.159245005384943</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.7568660021088933</v>
+        <v>0.7568660021065693</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.7581638448851888</v>
+        <v>0.7581638447191738</v>
       </c>
       <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="inlineStr"/>
@@ -1374,34 +1374,34 @@
       </c>
       <c r="AO7" t="inlineStr"/>
       <c r="AP7" t="n">
-        <v>3.516674491964692</v>
+        <v>3.516674488692475</v>
       </c>
       <c r="AQ7" t="n">
-        <v>3.670528190662636</v>
+        <v>3.6705281905585</v>
       </c>
       <c r="AR7" t="n">
-        <v>3.821603254287154</v>
+        <v>3.821603252977911</v>
       </c>
       <c r="AS7" t="n">
-        <v>3.885380516373269</v>
+        <v>3.885380512727744</v>
       </c>
       <c r="AT7" t="n">
-        <v>3.959648795689747</v>
+        <v>3.959648787425953</v>
       </c>
       <c r="AU7" t="n">
-        <v>0.6979970596618019</v>
+        <v>0.6979970594620387</v>
       </c>
       <c r="AV7" t="n">
-        <v>0.759272740940065</v>
+        <v>0.7592727409374319</v>
       </c>
       <c r="AW7" t="n">
-        <v>0.8321461482447932</v>
+        <v>0.8321461481383883</v>
       </c>
       <c r="AX7" t="n">
-        <v>0.8664197795581673</v>
+        <v>0.8664197792014181</v>
       </c>
       <c r="AY7" t="n">
-        <v>0.9067412904690462</v>
+        <v>0.9067412895450442</v>
       </c>
     </row>
     <row r="8">
@@ -1417,10 +1417,10 @@
         <v>0.1620698123117035</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.6431392381211656</v>
+        <v>-0.6431392374743101</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.6502050874688874</v>
+        <v>-0.6502050879872123</v>
       </c>
       <c r="L8" t="n">
         <v>293.15</v>
@@ -1432,10 +1432,10 @@
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="n">
-        <v>5.014323837139883</v>
+        <v>5.014323831714023</v>
       </c>
       <c r="T8" t="n">
-        <v>0.2899811531219729</v>
+        <v>0.2899811531093115</v>
       </c>
       <c r="U8" t="n">
         <v>293.15</v>
@@ -1453,13 +1453,13 @@
         <v>3.581884477099092</v>
       </c>
       <c r="Z8" t="n">
-        <v>3.562615766277579</v>
+        <v>3.562615763104827</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.7033324212463303</v>
+        <v>0.7033324212416372</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.7021575041703076</v>
+        <v>0.7021575039728042</v>
       </c>
       <c r="AC8" t="inlineStr"/>
       <c r="AD8" t="inlineStr"/>
@@ -1479,34 +1479,34 @@
       </c>
       <c r="AO8" t="inlineStr"/>
       <c r="AP8" t="n">
-        <v>3.213853783061053</v>
+        <v>3.213853779071183</v>
       </c>
       <c r="AQ8" t="n">
-        <v>3.361850238495738</v>
+        <v>3.361850237700157</v>
       </c>
       <c r="AR8" t="n">
-        <v>3.504525636639532</v>
+        <v>3.504525634909517</v>
       </c>
       <c r="AS8" t="n">
-        <v>3.563727769929077</v>
+        <v>3.563727766079489</v>
       </c>
       <c r="AT8" t="n">
-        <v>3.631702827130042</v>
+        <v>3.631702819046179</v>
       </c>
       <c r="AU8" t="n">
-        <v>0.6708954158405275</v>
+        <v>0.6708954156295289</v>
       </c>
       <c r="AV8" t="n">
-        <v>0.7250775140583019</v>
+        <v>0.725077514011906</v>
       </c>
       <c r="AW8" t="n">
-        <v>0.7890639816356142</v>
+        <v>0.7890639815104349</v>
       </c>
       <c r="AX8" t="n">
-        <v>0.8188065492218313</v>
+        <v>0.8188065488854981</v>
       </c>
       <c r="AY8" t="n">
-        <v>0.8531704781808276</v>
+        <v>0.8531704773580095</v>
       </c>
     </row>
     <row r="9">
@@ -1522,10 +1522,10 @@
         <v>0.223284760248648</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.785312103390047</v>
+        <v>-0.7853121027498691</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.7942185905573598</v>
+        <v>-0.7942185917021554</v>
       </c>
       <c r="L9" t="n">
         <v>293.15</v>
@@ -1537,10 +1537,10 @@
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="n">
-        <v>5.014323837139865</v>
+        <v>5.014323831714023</v>
       </c>
       <c r="T9" t="n">
-        <v>0.3199962481858906</v>
+        <v>0.3199962481604353</v>
       </c>
       <c r="U9" t="n">
         <v>293.15</v>
@@ -1558,13 +1558,13 @@
         <v>3.052743721168535</v>
       </c>
       <c r="Z9" t="n">
-        <v>3.030417126053114</v>
+        <v>3.03041712158862</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.6556339406748605</v>
+        <v>0.6556339406661077</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.6546080191529253</v>
+        <v>0.6546080189401164</v>
       </c>
       <c r="AC9" t="inlineStr"/>
       <c r="AD9" t="inlineStr"/>
@@ -1584,34 +1584,34 @@
       </c>
       <c r="AO9" t="inlineStr"/>
       <c r="AP9" t="n">
-        <v>2.957505713166264</v>
+        <v>2.957505708508922</v>
       </c>
       <c r="AQ9" t="n">
-        <v>3.098346825114579</v>
+        <v>3.098346823756458</v>
       </c>
       <c r="AR9" t="n">
-        <v>3.231623019756605</v>
+        <v>3.231623017807264</v>
       </c>
       <c r="AS9" t="n">
-        <v>3.285935618458844</v>
+        <v>3.28593561463626</v>
       </c>
       <c r="AT9" t="n">
-        <v>3.347359406904733</v>
+        <v>3.347359399254321</v>
       </c>
       <c r="AU9" t="n">
-        <v>0.6481242469577976</v>
+        <v>0.6481242467457952</v>
       </c>
       <c r="AV9" t="n">
-        <v>0.696303433121036</v>
+        <v>0.6963034330498501</v>
       </c>
       <c r="AW9" t="n">
-        <v>0.7527526603353999</v>
+        <v>0.7527526602143934</v>
       </c>
       <c r="AX9" t="n">
-        <v>0.7786439352948052</v>
+        <v>0.778643935001661</v>
       </c>
       <c r="AY9" t="n">
-        <v>0.807932998524012</v>
+        <v>0.8079329978220202</v>
       </c>
     </row>
     <row r="10">
@@ -1627,10 +1627,10 @@
         <v>0.3029631505528502</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.9204249302070969</v>
+        <v>-0.9204249295810688</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.9281692688409693</v>
+        <v>-0.9281692707362523</v>
       </c>
       <c r="L10" t="n">
         <v>293.15</v>
@@ -1642,10 +1642,10 @@
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="n">
-        <v>5.014323837139741</v>
+        <v>5.014323831714004</v>
       </c>
       <c r="T10" t="n">
-        <v>0.3779758311191301</v>
+        <v>0.3779758310661335</v>
       </c>
       <c r="U10" t="n">
         <v>293.15</v>
@@ -1663,13 +1663,13 @@
         <v>2.554509260158013</v>
       </c>
       <c r="Z10" t="n">
-        <v>2.536942856345228</v>
+        <v>2.536942850639571</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.6104858665364077</v>
+        <v>0.6104858665196271</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.609970857641253</v>
+        <v>0.6099708574584018</v>
       </c>
       <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="inlineStr"/>
@@ -1689,34 +1689,34 @@
       </c>
       <c r="AO10" t="inlineStr"/>
       <c r="AP10" t="n">
-        <v>2.739283315632882</v>
+        <v>2.739283310404228</v>
       </c>
       <c r="AQ10" t="n">
-        <v>2.872045099478158</v>
+        <v>2.872045097690081</v>
       </c>
       <c r="AR10" t="n">
-        <v>2.995184543148206</v>
+        <v>2.995184541133499</v>
       </c>
       <c r="AS10" t="n">
-        <v>3.044364886249034</v>
+        <v>3.044364882616229</v>
       </c>
       <c r="AT10" t="n">
-        <v>3.099022375814327</v>
+        <v>3.099022368757272</v>
       </c>
       <c r="AU10" t="n">
-        <v>0.628552623456151</v>
+        <v>0.6285526232533476</v>
       </c>
       <c r="AV10" t="n">
-        <v>0.6717073082429993</v>
+        <v>0.6717073081622922</v>
       </c>
       <c r="AW10" t="n">
-        <v>0.7218386769498653</v>
+        <v>0.721838676847632</v>
       </c>
       <c r="AX10" t="n">
-        <v>0.7444983536161848</v>
+        <v>0.7444983533782206</v>
       </c>
       <c r="AY10" t="n">
-        <v>0.7695255459836851</v>
+        <v>0.7695255454077957</v>
       </c>
     </row>
     <row r="11">
@@ -1732,10 +1732,10 @@
         <v>0.4005855232045683</v>
       </c>
       <c r="J11" t="n">
-        <v>-1.024429495805626</v>
+        <v>-1.024429495210301</v>
       </c>
       <c r="K11" t="n">
-        <v>-1.033323697841903</v>
+        <v>-1.033323700232518</v>
       </c>
       <c r="L11" t="n">
         <v>293.15</v>
@@ -1747,10 +1747,10 @@
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="n">
-        <v>5.014323837139632</v>
+        <v>5.014323831713982</v>
       </c>
       <c r="T11" t="n">
-        <v>0.4885231082909001</v>
+        <v>0.4885231081767439</v>
       </c>
       <c r="U11" t="n">
         <v>293.15</v>
@@ -1768,13 +1768,13 @@
         <v>2.142927524452521</v>
       </c>
       <c r="Z11" t="n">
-        <v>2.124731788996876</v>
+        <v>2.124731782907727</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.5700679870156936</v>
+        <v>0.5700679869825317</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.569858830273606</v>
+        <v>0.5698588301720074</v>
       </c>
       <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="inlineStr"/>
@@ -1794,34 +1794,34 @@
       </c>
       <c r="AO11" t="inlineStr"/>
       <c r="AP11" t="n">
-        <v>2.552258574624607</v>
+        <v>2.552258568951558</v>
       </c>
       <c r="AQ11" t="n">
-        <v>2.676381724291029</v>
+        <v>2.676381722204358</v>
       </c>
       <c r="AR11" t="n">
-        <v>2.788947117649769</v>
+        <v>2.788947115693118</v>
       </c>
       <c r="AS11" t="n">
-        <v>2.832858153771244</v>
+        <v>2.832858150438345</v>
       </c>
       <c r="AT11" t="n">
-        <v>2.880637629318183</v>
+        <v>2.880637622942425</v>
       </c>
       <c r="AU11" t="n">
-        <v>0.6113981980085841</v>
+        <v>0.611398197823776</v>
       </c>
       <c r="AV11" t="n">
-        <v>0.650412105074165</v>
+        <v>0.6504121049958466</v>
       </c>
       <c r="AW11" t="n">
-        <v>0.695333689558404</v>
+        <v>0.6953336894842983</v>
       </c>
       <c r="AX11" t="n">
-        <v>0.7153283048650831</v>
+        <v>0.715328304687297</v>
       </c>
       <c r="AY11" t="n">
-        <v>0.736841634677461</v>
+        <v>0.736841634224022</v>
       </c>
     </row>
     <row r="12">
@@ -1837,10 +1837,10 @@
         <v>0.5330711842725587</v>
       </c>
       <c r="J12" t="n">
-        <v>-1.095020728757032</v>
+        <v>-1.095020728247563</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.098870937940642</v>
+        <v>-1.098870939905237</v>
       </c>
       <c r="L12" t="n">
         <v>293.15</v>
@@ -1852,10 +1852,10 @@
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="n">
-        <v>5.014323837139724</v>
+        <v>5.01432383171401</v>
       </c>
       <c r="T12" t="n">
-        <v>0.747784957031429</v>
+        <v>0.7477849567407074</v>
       </c>
       <c r="U12" t="n">
         <v>293.15</v>
@@ -1873,13 +1873,13 @@
         <v>1.76278221600666</v>
       </c>
       <c r="Z12" t="n">
-        <v>1.755774599236958</v>
+        <v>1.755774594741567</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.5338950707383278</v>
+        <v>0.5338950706614285</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.5339660314658632</v>
+        <v>0.533966031435035</v>
       </c>
       <c r="AC12" t="inlineStr"/>
       <c r="AD12" t="inlineStr"/>
@@ -1899,34 +1899,34 @@
       </c>
       <c r="AO12" t="inlineStr"/>
       <c r="AP12" t="n">
-        <v>2.390751496751436</v>
+        <v>2.390751490780386</v>
       </c>
       <c r="AQ12" t="n">
-        <v>2.505992387141719</v>
+        <v>2.505992384884311</v>
       </c>
       <c r="AR12" t="n">
-        <v>2.607830719034865</v>
+        <v>2.607830717227307</v>
       </c>
       <c r="AS12" t="n">
-        <v>2.646446204237609</v>
+        <v>2.646446201272503</v>
       </c>
       <c r="AT12" t="n">
-        <v>2.687356072123862</v>
+        <v>2.687356066461796</v>
       </c>
       <c r="AU12" t="n">
-        <v>0.5961333103777453</v>
+        <v>0.5961333102175255</v>
       </c>
       <c r="AV12" t="n">
-        <v>0.6318126148868549</v>
+        <v>0.6318126148198606</v>
       </c>
       <c r="AW12" t="n">
-        <v>0.672540978847236</v>
+        <v>0.6725409788065138</v>
       </c>
       <c r="AX12" t="n">
-        <v>0.6903925288396244</v>
+        <v>0.6903925287225727</v>
       </c>
       <c r="AY12" t="n">
-        <v>0.7090837659471364</v>
+        <v>0.7090837656073812</v>
       </c>
     </row>
     <row r="13">
@@ -1942,10 +1942,10 @@
         <v>0.7231615990865421</v>
       </c>
       <c r="J13" t="n">
-        <v>-1.025706205147099</v>
+        <v>-1.025706204972748</v>
       </c>
       <c r="K13" t="n">
-        <v>-1.010849402518582</v>
+        <v>-1.010849402139139</v>
       </c>
       <c r="L13" t="n">
         <v>293.15</v>
@@ -1957,10 +1957,10 @@
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="n">
-        <v>5.014323837139645</v>
+        <v>5.014323831713992</v>
       </c>
       <c r="T13" t="n">
-        <v>1.545436856434068</v>
+        <v>1.545436855424525</v>
       </c>
       <c r="U13" t="n">
         <v>293.15</v>
@@ -1978,13 +1978,13 @@
         <v>1.41539264099721</v>
       </c>
       <c r="Z13" t="n">
-        <v>1.438623885919814</v>
+        <v>1.438623886245846</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.5424182014592162</v>
+        <v>0.5424182011993294</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.5416467498381698</v>
+        <v>0.5416467495669859</v>
       </c>
       <c r="AC13" t="inlineStr"/>
       <c r="AD13" t="inlineStr"/>
@@ -2004,34 +2004,34 @@
       </c>
       <c r="AO13" t="inlineStr"/>
       <c r="AP13" t="n">
-        <v>2.250153974250175</v>
+        <v>2.250153968138453</v>
       </c>
       <c r="AQ13" t="n">
-        <v>2.356524163954364</v>
+        <v>2.35652416164642</v>
       </c>
       <c r="AR13" t="n">
-        <v>2.447726512993743</v>
+        <v>2.447726511402287</v>
       </c>
       <c r="AS13" t="n">
-        <v>2.481121617856996</v>
+        <v>2.481121615294083</v>
       </c>
       <c r="AT13" t="n">
-        <v>2.515285590930509</v>
+        <v>2.515285585971907</v>
       </c>
       <c r="AU13" t="n">
-        <v>0.5824199281341085</v>
+        <v>0.5824199280024156</v>
       </c>
       <c r="AV13" t="n">
-        <v>0.6155097760840585</v>
+        <v>0.61550977603461</v>
       </c>
       <c r="AW13" t="n">
-        <v>0.6529894153393071</v>
+        <v>0.6529894153346865</v>
       </c>
       <c r="AX13" t="n">
-        <v>0.6691843963584141</v>
+        <v>0.6691843963001229</v>
       </c>
       <c r="AY13" t="n">
-        <v>0.6856994679804856</v>
+        <v>0.6856994677432419</v>
       </c>
     </row>
     <row r="14">
@@ -2047,10 +2047,10 @@
         <v>0.8465004587575707</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.7256658877045926</v>
+        <v>-0.7256658880749132</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.7484519615866625</v>
+        <v>-0.74845195995581</v>
       </c>
       <c r="L14" t="n">
         <v>293.15</v>
@@ -2062,10 +2062,10 @@
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="n">
-        <v>5.014323837139887</v>
+        <v>5.014323831714025</v>
       </c>
       <c r="T14" t="n">
-        <v>2.589746366583224</v>
+        <v>2.589746364404345</v>
       </c>
       <c r="U14" t="n">
         <v>293.15</v>
@@ -2083,13 +2083,13 @@
         <v>1.355411802377163</v>
       </c>
       <c r="Z14" t="n">
-        <v>1.322613325013736</v>
+        <v>1.322613327846136</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.6405128206399481</v>
+        <v>0.6405128199841453</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.6416088275445007</v>
+        <v>0.6416088267975284</v>
       </c>
       <c r="AC14" t="inlineStr"/>
       <c r="AD14" t="inlineStr"/>
@@ -2109,34 +2109,34 @@
       </c>
       <c r="AO14" t="inlineStr"/>
       <c r="AP14" t="n">
-        <v>2.126764219218889</v>
+        <v>2.126764213127873</v>
       </c>
       <c r="AQ14" t="n">
-        <v>2.224470111028816</v>
+        <v>2.224470108784999</v>
       </c>
       <c r="AR14" t="n">
-        <v>2.305325617563039</v>
+        <v>2.3053256162294</v>
       </c>
       <c r="AS14" t="n">
-        <v>2.333660165617131</v>
+        <v>2.333660163464161</v>
       </c>
       <c r="AT14" t="n">
-        <v>2.36130224401189</v>
+        <v>2.36130223971411</v>
       </c>
       <c r="AU14" t="n">
-        <v>0.5700643609044174</v>
+        <v>0.5700643608023055</v>
       </c>
       <c r="AV14" t="n">
-        <v>0.6012647675124257</v>
+        <v>0.6012647674844878</v>
       </c>
       <c r="AW14" t="n">
-        <v>0.6363871773819507</v>
+        <v>0.6363871774144002</v>
       </c>
       <c r="AX14" t="n">
-        <v>0.6513857040869248</v>
+        <v>0.6513857040843108</v>
       </c>
       <c r="AY14" t="n">
-        <v>0.666335919339722</v>
+        <v>0.6663359191933508</v>
       </c>
     </row>
     <row r="15">
@@ -2152,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0008760134604823555</v>
+        <v>0.0008760116297361065</v>
       </c>
       <c r="K15" t="n">
         <v>-0</v>
@@ -2167,10 +2167,10 @@
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="n">
-        <v>5.0143238371397</v>
+        <v>5.014323831714004</v>
       </c>
       <c r="T15" t="n">
-        <v>5.014323837139714</v>
+        <v>5.014323831714028</v>
       </c>
       <c r="U15" t="n">
         <v>293.15</v>
@@ -2188,13 +2188,13 @@
         <v>1.220882676837404</v>
       </c>
       <c r="Z15" t="n">
-        <v>1.219890078485025</v>
+        <v>1.219890080557699</v>
       </c>
       <c r="AA15" t="n">
-        <v>1.179590335194091</v>
+        <v>1.179590332263723</v>
       </c>
       <c r="AB15" t="n">
-        <v>1.179516417540028</v>
+        <v>1.179516414765168</v>
       </c>
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr"/>
@@ -2214,34 +2214,34 @@
       </c>
       <c r="AO15" t="inlineStr"/>
       <c r="AP15" t="n">
-        <v>2.017638355996423</v>
+        <v>2.017638350086308</v>
       </c>
       <c r="AQ15" t="n">
-        <v>2.107028293510612</v>
+        <v>2.107028291433338</v>
       </c>
       <c r="AR15" t="n">
-        <v>2.177976358022057</v>
+        <v>2.177976356973929</v>
       </c>
       <c r="AS15" t="n">
-        <v>2.201477403146879</v>
+        <v>2.201477401390479</v>
       </c>
       <c r="AT15" t="n">
-        <v>2.22290208526692</v>
+        <v>2.222902081563273</v>
       </c>
       <c r="AU15" t="n">
-        <v>0.5589859594634228</v>
+        <v>0.5589859593889961</v>
       </c>
       <c r="AV15" t="n">
-        <v>0.5889674717236711</v>
+        <v>0.5889674717191332</v>
       </c>
       <c r="AW15" t="n">
-        <v>0.6225901407367406</v>
+        <v>0.6225901408067239</v>
       </c>
       <c r="AX15" t="n">
-        <v>0.6368354401231023</v>
+        <v>0.636835440173075</v>
       </c>
       <c r="AY15" t="n">
-        <v>0.6508095535779259</v>
+        <v>0.6508095535117338</v>
       </c>
     </row>
     <row r="16">
@@ -2257,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.005897790957359983</v>
+        <v>-0.005897792266231536</v>
       </c>
       <c r="K16" t="n">
         <v>-0</v>
@@ -2272,7 +2272,7 @@
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="n">
-        <v>5.802519654320769</v>
+        <v>5.802519658302004</v>
       </c>
       <c r="T16" t="n">
         <v>0.3030841762674318</v>
@@ -2293,13 +2293,13 @@
         <v>6.277349563060453</v>
       </c>
       <c r="Z16" t="n">
-        <v>6.297792037214233</v>
+        <v>6.297792041754176</v>
       </c>
       <c r="AA16" t="n">
         <v>1.102127846664392</v>
       </c>
       <c r="AB16" t="n">
-        <v>1.105048531458197</v>
+        <v>1.105048532107958</v>
       </c>
       <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="inlineStr"/>
@@ -2319,34 +2319,34 @@
       </c>
       <c r="AO16" t="inlineStr"/>
       <c r="AP16" t="n">
-        <v>1.92046159666881</v>
+        <v>1.920461591093471</v>
       </c>
       <c r="AQ16" t="n">
-        <v>2.001979785353193</v>
+        <v>2.001979783533712</v>
       </c>
       <c r="AR16" t="n">
-        <v>2.063566637391407</v>
+        <v>2.063566636639104</v>
       </c>
       <c r="AS16" t="n">
-        <v>2.082510042588247</v>
+        <v>2.082510041198101</v>
       </c>
       <c r="AT16" t="n">
-        <v>2.098081515382115</v>
+        <v>2.09808151218905</v>
       </c>
       <c r="AU16" t="n">
-        <v>0.549196158489755</v>
+        <v>0.5491961584382158</v>
       </c>
       <c r="AV16" t="n">
-        <v>0.5786157973417358</v>
+        <v>0.5786157973608825</v>
       </c>
       <c r="AW16" t="n">
-        <v>0.6115821690505067</v>
+        <v>0.6115821691584502</v>
       </c>
       <c r="AX16" t="n">
-        <v>0.6255107942965484</v>
+        <v>0.6255107943968928</v>
       </c>
       <c r="AY16" t="n">
-        <v>0.6390885229496728</v>
+        <v>0.6390885229549566</v>
       </c>
     </row>
     <row r="17">
@@ -2362,10 +2362,10 @@
         <v>0.03137658994751866</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.1772643527698092</v>
+        <v>-0.1772643540781578</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.1694261339712823</v>
+        <v>-0.1694261341757806</v>
       </c>
       <c r="L17" t="n">
         <v>318.15</v>
@@ -2377,10 +2377,10 @@
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="n">
-        <v>5.802519654309018</v>
+        <v>5.802519658302006</v>
       </c>
       <c r="T17" t="n">
-        <v>0.3073376270346402</v>
+        <v>0.3073376270356393</v>
       </c>
       <c r="U17" t="n">
         <v>318.15</v>
@@ -2398,13 +2398,13 @@
         <v>5.591565228056824</v>
       </c>
       <c r="Z17" t="n">
-        <v>5.617404763140808</v>
+        <v>5.617404766783674</v>
       </c>
       <c r="AA17" t="n">
-        <v>1.000049546318908</v>
+        <v>1.000049546319431</v>
       </c>
       <c r="AB17" t="n">
-        <v>1.003282608842213</v>
+        <v>1.003282609299589</v>
       </c>
       <c r="AC17" t="inlineStr"/>
       <c r="AD17" t="inlineStr"/>
@@ -2424,34 +2424,34 @@
       </c>
       <c r="AO17" t="inlineStr"/>
       <c r="AP17" t="n">
-        <v>1.833437208682915</v>
+        <v>1.833437203585778</v>
       </c>
       <c r="AQ17" t="n">
-        <v>1.907584454649798</v>
+        <v>1.907584453165843</v>
       </c>
       <c r="AR17" t="n">
-        <v>1.960423425263066</v>
+        <v>1.960423424802918</v>
       </c>
       <c r="AS17" t="n">
-        <v>1.975116643014482</v>
+        <v>1.97511664194723</v>
       </c>
       <c r="AT17" t="n">
-        <v>1.98523796984644</v>
+        <v>1.985237967069519</v>
       </c>
       <c r="AU17" t="n">
-        <v>0.5407856550591027</v>
+        <v>0.5407856550229189</v>
       </c>
       <c r="AV17" t="n">
-        <v>0.5703040225634223</v>
+        <v>0.5703040226053514</v>
       </c>
       <c r="AW17" t="n">
-        <v>0.6034656787454631</v>
+        <v>0.6034656788925271</v>
       </c>
       <c r="AX17" t="n">
-        <v>0.6175192532297541</v>
+        <v>0.6175192533799071</v>
       </c>
       <c r="AY17" t="n">
-        <v>0.6312872308887667</v>
+        <v>0.6312872309595841</v>
       </c>
     </row>
     <row r="18">
@@ -2467,10 +2467,10 @@
         <v>0.069950087027647</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.3610904070420978</v>
+        <v>-0.3610904083493587</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.3501901728544622</v>
+        <v>-0.3501901733601814</v>
       </c>
       <c r="L18" t="n">
         <v>318.15</v>
@@ -2482,10 +2482,10 @@
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="n">
-        <v>5.802519654308991</v>
+        <v>5.80251965830202</v>
       </c>
       <c r="T18" t="n">
-        <v>0.315973267819829</v>
+        <v>0.3159732678228959</v>
       </c>
       <c r="U18" t="n">
         <v>318.15</v>
@@ -2503,13 +2503,13 @@
         <v>4.885311784854335</v>
       </c>
       <c r="Z18" t="n">
-        <v>4.919102915346276</v>
+        <v>4.919102917835361</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.905029273436572</v>
+        <v>0.9050292734380324</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.908663102761568</v>
+        <v>0.9086631030315816</v>
       </c>
       <c r="AC18" t="inlineStr"/>
       <c r="AD18" t="inlineStr"/>
@@ -2529,34 +2529,34 @@
       </c>
       <c r="AO18" t="inlineStr"/>
       <c r="AP18" t="n">
-        <v>1.755190712883971</v>
+        <v>1.755190708393733</v>
       </c>
       <c r="AQ18" t="n">
-        <v>1.822490550270154</v>
+        <v>1.822490549184201</v>
       </c>
       <c r="AR18" t="n">
-        <v>1.867226275592985</v>
+        <v>1.867226275408732</v>
       </c>
       <c r="AS18" t="n">
-        <v>1.877992169245442</v>
+        <v>1.877992168447626</v>
       </c>
       <c r="AT18" t="n">
-        <v>1.883085255632255</v>
+        <v>1.883085253171603</v>
       </c>
       <c r="AU18" t="n">
-        <v>0.5339186135907447</v>
+        <v>0.5339186135599132</v>
       </c>
       <c r="AV18" t="n">
-        <v>0.5642193646087371</v>
+        <v>0.5642193646718779</v>
       </c>
       <c r="AW18" t="n">
-        <v>0.5984622739542893</v>
+        <v>0.598462274143069</v>
       </c>
       <c r="AX18" t="n">
-        <v>0.6131017911280801</v>
+        <v>0.6131017913298401</v>
       </c>
       <c r="AY18" t="n">
-        <v>0.6276734622486942</v>
+        <v>0.627673462382469</v>
       </c>
     </row>
     <row r="19">
@@ -2572,10 +2572,10 @@
         <v>0.1108173186850926</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.516849774723972</v>
+        <v>-0.5168497760294796</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.5128098094113879</v>
+        <v>-0.5128098102683868</v>
       </c>
       <c r="L19" t="n">
         <v>318.15</v>
@@ -2587,10 +2587,10 @@
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="n">
-        <v>5.802519654308972</v>
+        <v>5.802519658302022</v>
       </c>
       <c r="T19" t="n">
-        <v>0.3293853879938005</v>
+        <v>0.3293853880001911</v>
       </c>
       <c r="U19" t="n">
         <v>318.15</v>
@@ -2608,13 +2608,13 @@
         <v>4.304441174639596</v>
       </c>
       <c r="Z19" t="n">
-        <v>4.316210206538743</v>
+        <v>4.316210207846297</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.8327397620341446</v>
+        <v>0.8327397620369507</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.8338309216450926</v>
+        <v>0.8338309217692847</v>
       </c>
       <c r="AC19" t="inlineStr"/>
       <c r="AD19" t="inlineStr"/>
@@ -2634,34 +2634,34 @@
       </c>
       <c r="AO19" t="inlineStr"/>
       <c r="AP19" t="n">
-        <v>1.68468619744568</v>
+        <v>1.68468619367275</v>
       </c>
       <c r="AQ19" t="n">
-        <v>1.745655112605398</v>
+        <v>1.745655111962874</v>
       </c>
       <c r="AR19" t="n">
-        <v>1.78293113786039</v>
+        <v>1.782931137924223</v>
       </c>
       <c r="AS19" t="n">
-        <v>1.790092969876655</v>
+        <v>1.790092969287411</v>
       </c>
       <c r="AT19" t="n">
-        <v>1.790579562334717</v>
+        <v>1.790579560089294</v>
       </c>
       <c r="AU19" t="n">
-        <v>0.5288336759870548</v>
+        <v>0.5288336759494522</v>
       </c>
       <c r="AV19" t="n">
-        <v>0.5606470148894442</v>
+        <v>0.5606470149721712</v>
       </c>
       <c r="AW19" t="n">
-        <v>0.5969243696646062</v>
+        <v>0.5969243698998935</v>
       </c>
       <c r="AX19" t="n">
-        <v>0.6126485296890067</v>
+        <v>0.6126485299472602</v>
       </c>
       <c r="AY19" t="n">
-        <v>0.6286901393266252</v>
+        <v>0.6286901395246364</v>
       </c>
     </row>
     <row r="20">
@@ -2677,10 +2677,10 @@
         <v>0.162296259598829</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.6769972937654185</v>
+        <v>-0.6769972950676608</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.6818848594610295</v>
+        <v>-0.681884860765215</v>
       </c>
       <c r="L20" t="n">
         <v>318.15</v>
@@ -2692,10 +2692,10 @@
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="n">
-        <v>5.802519654309203</v>
+        <v>5.802519658302032</v>
       </c>
       <c r="T20" t="n">
-        <v>0.3530414408547867</v>
+        <v>0.3530414408673431</v>
       </c>
       <c r="U20" t="n">
         <v>318.15</v>
@@ -2713,13 +2713,13 @@
         <v>3.728050506136204</v>
       </c>
       <c r="Z20" t="n">
-        <v>3.714835053041543</v>
+        <v>3.714835053036312</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.7652651520584984</v>
+        <v>0.7652651520635652</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.7642430955176571</v>
+        <v>0.7642430955223128</v>
       </c>
       <c r="AC20" t="inlineStr"/>
       <c r="AD20" t="inlineStr"/>
@@ -2739,34 +2739,34 @@
       </c>
       <c r="AO20" t="inlineStr"/>
       <c r="AP20" t="n">
-        <v>1.621151789623175</v>
+        <v>1.621151786655864</v>
       </c>
       <c r="AQ20" t="n">
-        <v>1.676272560976504</v>
+        <v>1.676272560804195</v>
       </c>
       <c r="AR20" t="n">
-        <v>1.706701944323127</v>
+        <v>1.706701944596718</v>
       </c>
       <c r="AS20" t="n">
-        <v>1.710569547295547</v>
+        <v>1.710569546848714</v>
       </c>
       <c r="AT20" t="n">
-        <v>1.706853462159178</v>
+        <v>1.706853460031485</v>
       </c>
       <c r="AU20" t="n">
-        <v>0.5258523990332419</v>
+        <v>0.5258523989750445</v>
       </c>
       <c r="AV20" t="n">
-        <v>0.5599849179116525</v>
+        <v>0.5599849180130047</v>
       </c>
       <c r="AW20" t="n">
-        <v>0.5993601293876298</v>
+        <v>0.5993601296773079</v>
       </c>
       <c r="AX20" t="n">
-        <v>0.6167298386206356</v>
+        <v>0.6167298389441728</v>
       </c>
       <c r="AY20" t="n">
-        <v>0.6349956820530892</v>
+        <v>0.6349956823209827</v>
       </c>
     </row>
     <row r="21">
@@ -2782,10 +2782,10 @@
         <v>0.2250238576876559</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.8430752646660493</v>
+        <v>-0.8430752659623351</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.8440320745737692</v>
+        <v>-0.8440320763664155</v>
       </c>
       <c r="L21" t="n">
         <v>318.15</v>
@@ -2797,10 +2797,10 @@
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="n">
-        <v>5.802519654309125</v>
+        <v>5.802519658302002</v>
       </c>
       <c r="T21" t="n">
-        <v>0.3935127175501378</v>
+        <v>0.3935127175740876</v>
       </c>
       <c r="U21" t="n">
         <v>318.15</v>
@@ -2818,13 +2818,13 @@
         <v>3.162639207822131</v>
       </c>
       <c r="Z21" t="n">
-        <v>3.160268067545646</v>
+        <v>3.160268066315895</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.7031895028496933</v>
+        <v>0.7031895028585389</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.7030440936950038</v>
+        <v>0.7030440936284622</v>
       </c>
       <c r="AC21" t="inlineStr"/>
       <c r="AD21" t="inlineStr"/>
@@ -2844,34 +2844,34 @@
       </c>
       <c r="AO21" t="inlineStr"/>
       <c r="AP21" t="n">
-        <v>1.564011727652123</v>
+        <v>1.564011725553571</v>
       </c>
       <c r="AQ21" t="n">
-        <v>1.613709317965362</v>
+        <v>1.613709318269645</v>
       </c>
       <c r="AR21" t="n">
-        <v>1.637848136823931</v>
+        <v>1.637848137259166</v>
       </c>
       <c r="AS21" t="n">
-        <v>1.638705393594831</v>
+        <v>1.638705393221614</v>
       </c>
       <c r="AT21" t="n">
-        <v>1.631156298966765</v>
+        <v>1.631156296866179</v>
       </c>
       <c r="AU21" t="n">
-        <v>0.525396677542736</v>
+        <v>0.5253966774488547</v>
       </c>
       <c r="AV21" t="n">
-        <v>0.5627708459220253</v>
+        <v>0.562770846042567</v>
       </c>
       <c r="AW21" t="n">
-        <v>0.6064758971706213</v>
+        <v>0.6064758975267638</v>
       </c>
       <c r="AX21" t="n">
-        <v>0.6261480793852374</v>
+        <v>0.6261480797877856</v>
       </c>
       <c r="AY21" t="n">
-        <v>0.6475297694410279</v>
+        <v>0.647529769789403</v>
       </c>
     </row>
     <row r="22">
@@ -2887,10 +2887,10 @@
         <v>0.3043733133467496</v>
       </c>
       <c r="J22" t="n">
-        <v>-1.003266220244825</v>
+        <v>-1.003266221529155</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.9959190110692675</v>
+        <v>-0.9959190132950994</v>
       </c>
       <c r="L22" t="n">
         <v>318.15</v>
@@ -2902,10 +2902,10 @@
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="n">
-        <v>5.802519654309165</v>
+        <v>5.802519658302019</v>
       </c>
       <c r="T22" t="n">
-        <v>0.4673458917519175</v>
+        <v>0.4673458917990946</v>
       </c>
       <c r="U22" t="n">
         <v>318.15</v>
@@ -2923,13 +2923,13 @@
         <v>2.636211180420427</v>
       </c>
       <c r="Z22" t="n">
-        <v>2.652689254614053</v>
+        <v>2.652689252498005</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.6471060694882199</v>
+        <v>0.6471060695040926</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.6478286414181456</v>
+        <v>0.6478286413408769</v>
       </c>
       <c r="AC22" t="inlineStr"/>
       <c r="AD22" t="inlineStr"/>
@@ -2949,34 +2949,34 @@
       </c>
       <c r="AO22" t="inlineStr"/>
       <c r="AP22" t="n">
-        <v>1.512823003737896</v>
+        <v>1.512823002542796</v>
       </c>
       <c r="AQ22" t="n">
-        <v>1.557442954043602</v>
+        <v>1.557442954808621</v>
       </c>
       <c r="AR22" t="n">
-        <v>1.575767080956322</v>
+        <v>1.575767081496139</v>
       </c>
       <c r="AS22" t="n">
-        <v>1.5738610439966</v>
+        <v>1.573861043626962</v>
       </c>
       <c r="AT22" t="n">
-        <v>1.562800392617966</v>
+        <v>1.562800390464541</v>
       </c>
       <c r="AU22" t="n">
-        <v>0.5280179219306328</v>
+        <v>0.528017921785111</v>
       </c>
       <c r="AV22" t="n">
-        <v>0.5697260965280534</v>
+        <v>0.5697260966708881</v>
       </c>
       <c r="AW22" t="n">
-        <v>0.619243050844139</v>
+        <v>0.619243051284453</v>
       </c>
       <c r="AX22" t="n">
-        <v>0.6420185697074666</v>
+        <v>0.6420185702090637</v>
       </c>
       <c r="AY22" t="n">
-        <v>0.6676156729931397</v>
+        <v>0.6676156734384201</v>
       </c>
     </row>
     <row r="23">
@@ -2992,10 +2992,10 @@
         <v>0.4036681690445971</v>
       </c>
       <c r="J23" t="n">
-        <v>-1.131557241394679</v>
+        <v>-1.131557242653062</v>
       </c>
       <c r="K23" t="n">
-        <v>-1.123726229948751</v>
+        <v>-1.123726232308614</v>
       </c>
       <c r="L23" t="n">
         <v>318.15</v>
@@ -3007,10 +3007,10 @@
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="n">
-        <v>5.802519654309119</v>
+        <v>5.802519658302023</v>
       </c>
       <c r="T23" t="n">
-        <v>0.6083022994666517</v>
+        <v>0.6083022995654389</v>
       </c>
       <c r="U23" t="n">
         <v>318.15</v>
@@ -3028,13 +3028,13 @@
         <v>2.195064137080933</v>
       </c>
       <c r="Z23" t="n">
-        <v>2.21087542990112</v>
+        <v>2.210875427671152</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.5994250733792564</v>
+        <v>0.5994250734095171</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.5998170405212377</v>
+        <v>0.5998170404958324</v>
       </c>
       <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="inlineStr"/>
@@ -3054,34 +3054,34 @@
       </c>
       <c r="AO23" t="inlineStr"/>
       <c r="AP23" t="n">
-        <v>1.467215181228073</v>
+        <v>1.467215180939795</v>
       </c>
       <c r="AQ23" t="n">
-        <v>1.507004989663924</v>
+        <v>1.507004990850977</v>
       </c>
       <c r="AR23" t="n">
-        <v>1.519891152426549</v>
+        <v>1.519891153006271</v>
       </c>
       <c r="AS23" t="n">
-        <v>1.515423453365779</v>
+        <v>1.515423452930597</v>
       </c>
       <c r="AT23" t="n">
-        <v>1.50111353963441</v>
+        <v>1.501113537361864</v>
       </c>
       <c r="AU23" t="n">
-        <v>0.5344425124113785</v>
+        <v>0.534442512197654</v>
       </c>
       <c r="AV23" t="n">
-        <v>0.5818228402871214</v>
+        <v>0.5818228404591037</v>
       </c>
       <c r="AW23" t="n">
-        <v>0.639000536608596</v>
+        <v>0.6390005371584051</v>
       </c>
       <c r="AX23" t="n">
-        <v>0.6658937461508702</v>
+        <v>0.6658937467798585</v>
       </c>
       <c r="AY23" t="n">
-        <v>0.6971174447986175</v>
+        <v>0.6971174453644242</v>
       </c>
     </row>
     <row r="24">
@@ -3097,10 +3097,10 @@
         <v>0.5352323278264397</v>
       </c>
       <c r="J24" t="n">
-        <v>-1.207488682885183</v>
+        <v>-1.207488684074334</v>
       </c>
       <c r="K24" t="n">
-        <v>-1.207024443036532</v>
+        <v>-1.207024444815176</v>
       </c>
       <c r="L24" t="n">
         <v>318.15</v>
@@ -3112,10 +3112,10 @@
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="n">
-        <v>5.802519654309197</v>
+        <v>5.802519658302022</v>
       </c>
       <c r="T24" t="n">
-        <v>0.9246061100634994</v>
+        <v>0.9246061103038871</v>
       </c>
       <c r="U24" t="n">
         <v>318.15</v>
@@ -3133,13 +3133,13 @@
         <v>1.81706432362279</v>
       </c>
       <c r="Z24" t="n">
-        <v>1.817899913719612</v>
+        <v>1.817899912658228</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.5639426515466207</v>
+        <v>0.5639426516141204</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.5639451528351173</v>
+        <v>0.5639451528994329</v>
       </c>
       <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr"/>
@@ -3159,34 +3159,34 @@
       </c>
       <c r="AO24" t="inlineStr"/>
       <c r="AP24" t="n">
-        <v>1.426832821317666</v>
+        <v>1.426832821906077</v>
       </c>
       <c r="AQ24" t="n">
-        <v>1.461927741580387</v>
+        <v>1.461927743125391</v>
       </c>
       <c r="AR24" t="n">
-        <v>1.469640492253621</v>
+        <v>1.469640492799201</v>
       </c>
       <c r="AS24" t="n">
-        <v>1.462761837887772</v>
+        <v>1.462761837320629</v>
       </c>
       <c r="AT24" t="n">
-        <v>1.445399408656647</v>
+        <v>1.445399406214918</v>
       </c>
       <c r="AU24" t="n">
-        <v>0.5456407891944195</v>
+        <v>0.5456407888952797</v>
       </c>
       <c r="AV24" t="n">
-        <v>0.6003864744878155</v>
+        <v>0.6003864747010701</v>
       </c>
       <c r="AW24" t="n">
-        <v>0.6676114706514877</v>
+        <v>0.6676114713465638</v>
       </c>
       <c r="AX24" t="n">
-        <v>0.699953468215612</v>
+        <v>0.6999534690116183</v>
       </c>
       <c r="AY24" t="n">
-        <v>0.7386821980498639</v>
+        <v>0.7386821987692849</v>
       </c>
     </row>
     <row r="25">
@@ -3202,10 +3202,10 @@
         <v>0.7231615990865421</v>
       </c>
       <c r="J25" t="n">
-        <v>-1.126923768366777</v>
+        <v>-1.126923769299651</v>
       </c>
       <c r="K25" t="n">
-        <v>-1.115477915804471</v>
+        <v>-1.115477915799007</v>
       </c>
       <c r="L25" t="n">
         <v>318.15</v>
@@ -3217,10 +3217,10 @@
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="n">
-        <v>5.802519654309146</v>
+        <v>5.802519658302005</v>
       </c>
       <c r="T25" t="n">
-        <v>1.860682863646959</v>
+        <v>1.860682864434041</v>
       </c>
       <c r="U25" t="n">
         <v>318.15</v>
@@ -3238,13 +3238,13 @@
         <v>1.457611600894914</v>
       </c>
       <c r="Z25" t="n">
-        <v>1.475144301351317</v>
+        <v>1.47514430279581</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.5942417489417255</v>
+        <v>0.5942417491651432</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.5939383163234928</v>
+        <v>0.5939383165225308</v>
       </c>
       <c r="AC25" t="inlineStr"/>
       <c r="AD25" t="inlineStr"/>
@@ -3264,34 +3264,34 @@
       </c>
       <c r="AO25" t="inlineStr"/>
       <c r="AP25" t="n">
-        <v>1.391280709946804</v>
+        <v>1.391280711344183</v>
       </c>
       <c r="AQ25" t="n">
-        <v>1.421696099463673</v>
+        <v>1.421696101277219</v>
       </c>
       <c r="AR25" t="n">
-        <v>1.42438335104918</v>
+        <v>1.424383351482622</v>
       </c>
       <c r="AS25" t="n">
-        <v>1.415192559990422</v>
+        <v>1.415192559229643</v>
       </c>
       <c r="AT25" t="n">
-        <v>1.39490856350577</v>
+        <v>1.394908560863701</v>
       </c>
       <c r="AU25" t="n">
-        <v>0.562931330920857</v>
+        <v>0.5629313305179762</v>
       </c>
       <c r="AV25" t="n">
-        <v>0.6272515631273796</v>
+        <v>0.6272515634012095</v>
       </c>
       <c r="AW25" t="n">
-        <v>0.7077042604353889</v>
+        <v>0.7077042613261652</v>
       </c>
       <c r="AX25" t="n">
-        <v>0.747299722313681</v>
+        <v>0.7472997233322296</v>
       </c>
       <c r="AY25" t="n">
-        <v>0.796118353442429</v>
+        <v>0.7961183543618409</v>
       </c>
     </row>
     <row r="26">
@@ -3307,10 +3307,10 @@
         <v>0.8465004587575707</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.8231264137356284</v>
+        <v>-0.823126414269244</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.8233171012664426</v>
+        <v>-0.823317100369387</v>
       </c>
       <c r="L26" t="n">
         <v>318.15</v>
@@ -3322,10 +3322,10 @@
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="n">
-        <v>5.802519654309138</v>
+        <v>5.802519658301984</v>
       </c>
       <c r="T26" t="n">
-        <v>3.065861241564743</v>
+        <v>3.065861243218506</v>
       </c>
       <c r="U26" t="n">
         <v>318.15</v>
@@ -3343,13 +3343,13 @@
         <v>1.341472116628346</v>
       </c>
       <c r="Z26" t="n">
-        <v>1.341213132343108</v>
+        <v>1.341213134285977</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.7431680786806408</v>
+        <v>0.7431680792567594</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.743169851724972</v>
+        <v>0.7431698522877774</v>
       </c>
       <c r="AC26" t="inlineStr"/>
       <c r="AD26" t="inlineStr"/>
@@ -3369,34 +3369,34 @@
       </c>
       <c r="AO26" t="inlineStr"/>
       <c r="AP26" t="n">
-        <v>1.360074763224271</v>
+        <v>1.360074765325691</v>
       </c>
       <c r="AQ26" t="n">
-        <v>1.385707678888458</v>
+        <v>1.38570768085549</v>
       </c>
       <c r="AR26" t="n">
-        <v>1.383407444268951</v>
+        <v>1.383407444507483</v>
       </c>
       <c r="AS26" t="n">
-        <v>1.371956300155578</v>
+        <v>1.371956299146446</v>
       </c>
       <c r="AT26" t="n">
-        <v>1.348823820400205</v>
+        <v>1.348823817547343</v>
       </c>
       <c r="AU26" t="n">
-        <v>0.5881397996132905</v>
+        <v>0.5881397990857989</v>
       </c>
       <c r="AV26" t="n">
-        <v>0.6650022582066808</v>
+        <v>0.665002258570105</v>
       </c>
       <c r="AW26" t="n">
-        <v>0.7630496448533318</v>
+        <v>0.7630496460113039</v>
       </c>
       <c r="AX26" t="n">
-        <v>0.8124207649877916</v>
+        <v>0.812420766307592</v>
       </c>
       <c r="AY26" t="n">
-        <v>0.8749972152430495</v>
+        <v>0.8749972164285845</v>
       </c>
     </row>
     <row r="27">
@@ -3412,7 +3412,7 @@
         <v>1</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.002902826488331955</v>
+        <v>-0.002902825973632561</v>
       </c>
       <c r="K27" t="n">
         <v>-0</v>
@@ -3427,10 +3427,10 @@
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="n">
-        <v>5.802519654308239</v>
+        <v>5.802519658301994</v>
       </c>
       <c r="T27" t="n">
-        <v>5.802519654308237</v>
+        <v>5.802519658302004</v>
       </c>
       <c r="U27" t="n">
         <v>318.15</v>
@@ -3448,13 +3448,13 @@
         <v>1.209106506564844</v>
       </c>
       <c r="Z27" t="n">
-        <v>1.212110986849986</v>
+        <v>1.21211098631514</v>
       </c>
       <c r="AA27" t="n">
-        <v>1.528332300507447</v>
+        <v>1.528332303295038</v>
       </c>
       <c r="AB27" t="n">
-        <v>1.528975913157299</v>
+        <v>1.528975915833775</v>
       </c>
       <c r="AC27" t="inlineStr"/>
       <c r="AD27" t="inlineStr"/>
@@ -3474,34 +3474,34 @@
       </c>
       <c r="AO27" t="inlineStr"/>
       <c r="AP27" t="n">
-        <v>1.332601125927544</v>
+        <v>1.332601128587931</v>
       </c>
       <c r="AQ27" t="n">
-        <v>1.353245408231211</v>
+        <v>1.353245410211086</v>
       </c>
       <c r="AR27" t="n">
-        <v>1.345907613771808</v>
+        <v>1.345907613730958</v>
       </c>
       <c r="AS27" t="n">
-        <v>1.332212688173526</v>
+        <v>1.332212686871227</v>
       </c>
       <c r="AT27" t="n">
-        <v>1.306264084136712</v>
+        <v>1.306264081084509</v>
       </c>
       <c r="AU27" t="n">
-        <v>0.6238447836507259</v>
+        <v>0.6238447829725174</v>
       </c>
       <c r="AV27" t="n">
-        <v>0.7173496720189639</v>
+        <v>0.7173496725141909</v>
       </c>
       <c r="AW27" t="n">
-        <v>0.8391622670683179</v>
+        <v>0.839162268596042</v>
       </c>
       <c r="AX27" t="n">
-        <v>0.9019377486714837</v>
+        <v>0.9019377504062107</v>
       </c>
       <c r="AY27" t="n">
-        <v>0.9836313546793481</v>
+        <v>0.9836313562280337</v>
       </c>
     </row>
     <row r="28">
@@ -3517,7 +3517,7 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.0001021667367517298</v>
+        <v>-0.0001021685422384622</v>
       </c>
       <c r="K28" t="n">
         <v>-0</v>
@@ -3532,7 +3532,7 @@
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="n">
-        <v>6.796093401777894</v>
+        <v>6.796093411600402</v>
       </c>
       <c r="T28" t="n">
         <v>0.3581104406685798</v>
@@ -3553,13 +3553,13 @@
         <v>6.493517115399269</v>
       </c>
       <c r="Z28" t="n">
-        <v>6.493884278167967</v>
+        <v>6.493884284656567</v>
       </c>
       <c r="AA28" t="n">
         <v>1.246925138207635</v>
       </c>
       <c r="AB28" t="n">
-        <v>1.246982030915516</v>
+        <v>1.246982031920959</v>
       </c>
       <c r="AC28" t="inlineStr"/>
       <c r="AD28" t="inlineStr"/>
@@ -3579,34 +3579,34 @@
       </c>
       <c r="AO28" t="inlineStr"/>
       <c r="AP28" t="n">
-        <v>1.308091407308378</v>
+        <v>1.308091410342944</v>
       </c>
       <c r="AQ28" t="n">
-        <v>1.323469860837713</v>
+        <v>1.323469862670515</v>
       </c>
       <c r="AR28" t="n">
-        <v>1.310994640432197</v>
+        <v>1.310994640030226</v>
       </c>
       <c r="AS28" t="n">
-        <v>1.29505636001015</v>
+        <v>1.295056358381017</v>
       </c>
       <c r="AT28" t="n">
-        <v>1.266310110454745</v>
+        <v>1.266310107236731</v>
       </c>
       <c r="AU28" t="n">
-        <v>0.6737660346251692</v>
+        <v>0.673766033759737</v>
       </c>
       <c r="AV28" t="n">
-        <v>0.789737191581842</v>
+        <v>0.7897371922690257</v>
       </c>
       <c r="AW28" t="n">
-        <v>0.9442831155209392</v>
+        <v>0.9442831175679582</v>
       </c>
       <c r="AX28" t="n">
-        <v>1.025834975256883</v>
+        <v>1.025834977574512</v>
       </c>
       <c r="AY28" t="n">
-        <v>1.134706201785194</v>
+        <v>1.134706203844529</v>
       </c>
     </row>
     <row r="29">
@@ -3622,10 +3622,10 @@
         <v>0.03147756134740528</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.1756356239639192</v>
+        <v>-0.1756356257673375</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.1753503738823323</v>
+        <v>-0.1753503745135355</v>
       </c>
       <c r="L29" t="n">
         <v>348.15</v>
@@ -3637,10 +3637,10 @@
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="n">
-        <v>6.7960934017776</v>
+        <v>6.796093411600426</v>
       </c>
       <c r="T29" t="n">
-        <v>0.3660694662875814</v>
+        <v>0.3660694662915324</v>
       </c>
       <c r="U29" t="n">
         <v>348.15</v>
@@ -3658,13 +3658,13 @@
         <v>5.795186518078085</v>
       </c>
       <c r="Z29" t="n">
-        <v>5.796145468317544</v>
+        <v>5.796145472258677</v>
       </c>
       <c r="AA29" t="n">
-        <v>1.128471304121047</v>
+        <v>1.12847130412338</v>
       </c>
       <c r="AB29" t="n">
-        <v>1.12860647635855</v>
+        <v>1.128606476916451</v>
       </c>
       <c r="AC29" t="inlineStr"/>
       <c r="AD29" t="inlineStr"/>
@@ -3684,34 +3684,34 @@
       </c>
       <c r="AO29" t="inlineStr"/>
       <c r="AP29" t="n">
-        <v>1.285622166707688</v>
+        <v>1.285622169894622</v>
       </c>
       <c r="AQ29" t="n">
-        <v>1.295437606175564</v>
+        <v>1.295437607682898</v>
       </c>
       <c r="AR29" t="n">
-        <v>1.277730201306819</v>
+        <v>1.277730200468864</v>
       </c>
       <c r="AS29" t="n">
-        <v>1.259558864896603</v>
+        <v>1.259558862923347</v>
       </c>
       <c r="AT29" t="n">
-        <v>1.228053102255806</v>
+        <v>1.228053098926207</v>
       </c>
       <c r="AU29" t="n">
-        <v>0.7433921553891859</v>
+        <v>0.7433921542800125</v>
       </c>
       <c r="AV29" t="n">
-        <v>0.8903353582253662</v>
+        <v>0.8903353591891884</v>
       </c>
       <c r="AW29" t="n">
-        <v>1.091025674627499</v>
+        <v>1.091025677416207</v>
       </c>
       <c r="AX29" t="n">
-        <v>1.199541284843725</v>
+        <v>1.199541287999475</v>
       </c>
       <c r="AY29" t="n">
-        <v>1.34807628268811</v>
+        <v>1.348076285491559</v>
       </c>
     </row>
     <row r="30">
@@ -3727,10 +3727,10 @@
         <v>0.06769199592074771</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.3566666042460545</v>
+        <v>-0.356666606046077</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.3533058217018913</v>
+        <v>-0.3533058229331914</v>
       </c>
       <c r="L30" t="n">
         <v>348.15</v>
@@ -3742,10 +3742,10 @@
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="n">
-        <v>6.796093401777624</v>
+        <v>6.796093411600403</v>
       </c>
       <c r="T30" t="n">
-        <v>0.3786921200729297</v>
+        <v>0.3786921200833214</v>
       </c>
       <c r="U30" t="n">
         <v>348.15</v>
@@ -3763,13 +3763,13 @@
         <v>5.116758403120961</v>
       </c>
       <c r="Z30" t="n">
-        <v>5.127287669420581</v>
+        <v>5.12728767120351</v>
       </c>
       <c r="AA30" t="n">
-        <v>1.020764753682342</v>
+        <v>1.020764753687917</v>
       </c>
       <c r="AB30" t="n">
-        <v>1.022097773557331</v>
+        <v>1.02209777378879</v>
       </c>
       <c r="AC30" t="inlineStr"/>
       <c r="AD30" t="inlineStr"/>
@@ -3789,34 +3789,34 @@
       </c>
       <c r="AO30" t="inlineStr"/>
       <c r="AP30" t="n">
-        <v>1.264148358922106</v>
+        <v>1.264148362009051</v>
       </c>
       <c r="AQ30" t="n">
-        <v>1.268152368359357</v>
+        <v>1.268152369357286</v>
       </c>
       <c r="AR30" t="n">
-        <v>1.245189655530751</v>
+        <v>1.245189654195187</v>
       </c>
       <c r="AS30" t="n">
-        <v>1.224833867037365</v>
+        <v>1.22483386471994</v>
       </c>
       <c r="AT30" t="n">
-        <v>1.190662256723742</v>
+        <v>1.190662253354169</v>
       </c>
       <c r="AU30" t="n">
-        <v>0.8410216095336533</v>
+        <v>0.8410216080860268</v>
       </c>
       <c r="AV30" t="n">
-        <v>1.031720687678678</v>
+        <v>1.031720689036772</v>
       </c>
       <c r="AW30" t="n">
-        <v>1.29921179162278</v>
+        <v>1.299211795491453</v>
       </c>
       <c r="AX30" t="n">
-        <v>1.447552998742947</v>
+        <v>1.447553003136399</v>
       </c>
       <c r="AY30" t="n">
-        <v>1.655700743177297</v>
+        <v>1.655700747110892</v>
       </c>
     </row>
     <row r="31">
@@ -3832,10 +3832,10 @@
         <v>0.1113805678168688</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.5494216361961132</v>
+        <v>-0.5494216379903829</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.538343670113272</v>
+        <v>-0.5383436719050658</v>
       </c>
       <c r="L31" t="n">
         <v>348.15</v>
@@ -3847,10 +3847,10 @@
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="n">
-        <v>6.7960934017776</v>
+        <v>6.796093411600432</v>
       </c>
       <c r="T31" t="n">
-        <v>0.3991687052807046</v>
+        <v>0.3991687053019809</v>
       </c>
       <c r="U31" t="n">
         <v>348.15</v>
@@ -3868,13 +3868,13 @@
         <v>4.439297158405888</v>
       </c>
       <c r="Z31" t="n">
-        <v>4.471390282515214</v>
+        <v>4.471390282522425</v>
       </c>
       <c r="AA31" t="n">
-        <v>0.9203490221029574</v>
+        <v>0.9203490221132787</v>
       </c>
       <c r="AB31" t="n">
-        <v>0.923921913251025</v>
+        <v>0.9239219132621899</v>
       </c>
       <c r="AC31" t="inlineStr"/>
       <c r="AD31" t="inlineStr"/>
@@ -3894,34 +3894,34 @@
       </c>
       <c r="AO31" t="inlineStr"/>
       <c r="AP31" t="n">
-        <v>1.242578364177125</v>
+        <v>1.242578366893038</v>
       </c>
       <c r="AQ31" t="n">
-        <v>1.240650495309107</v>
+        <v>1.240650495619164</v>
       </c>
       <c r="AR31" t="n">
-        <v>1.212547209006202</v>
+        <v>1.212547207132182</v>
       </c>
       <c r="AS31" t="n">
-        <v>1.190119719726198</v>
+        <v>1.190119717083555</v>
       </c>
       <c r="AT31" t="n">
-        <v>1.153460919994332</v>
+        <v>1.153460916668255</v>
       </c>
       <c r="AU31" t="n">
-        <v>0.9795367918069717</v>
+        <v>0.9795367898525151</v>
       </c>
       <c r="AV31" t="n">
-        <v>1.233790020315068</v>
+        <v>1.233790022227438</v>
       </c>
       <c r="AW31" t="n">
-        <v>1.600905154897833</v>
+        <v>1.600905160374254</v>
       </c>
       <c r="AX31" t="n">
-        <v>1.809936667463979</v>
+        <v>1.809936673742017</v>
       </c>
       <c r="AY31" t="n">
-        <v>2.110635786550984</v>
+        <v>2.11063579228345</v>
       </c>
     </row>
     <row r="32">
@@ -3937,10 +3937,10 @@
         <v>0.1621264073004131</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.7225087563550985</v>
+        <v>-0.7225087581399378</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.7186167861001067</v>
+        <v>-0.7186167883435098</v>
       </c>
       <c r="L32" t="n">
         <v>348.15</v>
@@ -3952,10 +3952,10 @@
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="n">
-        <v>6.796093401777464</v>
+        <v>6.796093411600435</v>
       </c>
       <c r="T32" t="n">
-        <v>0.430909424294911</v>
+        <v>0.4309094243340721</v>
       </c>
       <c r="U32" t="n">
         <v>348.15</v>
@@ -3973,13 +3973,13 @@
         <v>3.858292628346104</v>
       </c>
       <c r="Z32" t="n">
-        <v>3.86870879135814</v>
+        <v>3.868708790129848</v>
       </c>
       <c r="AA32" t="n">
-        <v>0.8376326919456988</v>
+        <v>0.8376326919629996</v>
       </c>
       <c r="AB32" t="n">
-        <v>0.83863500056308</v>
+        <v>0.838635000462097</v>
       </c>
       <c r="AC32" t="inlineStr"/>
       <c r="AD32" t="inlineStr"/>
@@ -3999,34 +3999,34 @@
       </c>
       <c r="AO32" t="inlineStr"/>
       <c r="AP32" t="n">
-        <v>1.219890078485025</v>
+        <v>1.219890080557699</v>
       </c>
       <c r="AQ32" t="n">
-        <v>1.212110986849986</v>
+        <v>1.21211098631514</v>
       </c>
       <c r="AR32" t="n">
-        <v>1.179170144643762</v>
+        <v>1.179170142169031</v>
       </c>
       <c r="AS32" t="n">
-        <v>1.154863361315</v>
+        <v>1.154863358384558</v>
       </c>
       <c r="AT32" t="n">
-        <v>1.115995056017709</v>
+        <v>1.115995052823134</v>
       </c>
       <c r="AU32" t="n">
-        <v>1.1795164175401</v>
+        <v>1.179516414765168</v>
       </c>
       <c r="AV32" t="n">
-        <v>1.528975913158662</v>
+        <v>1.528975915833789</v>
       </c>
       <c r="AW32" t="n">
-        <v>2.049637537130585</v>
+        <v>2.049637545037952</v>
       </c>
       <c r="AX32" t="n">
-        <v>2.354392846903091</v>
+        <v>2.354392856152201</v>
       </c>
       <c r="AY32" t="n">
-        <v>2.803989055296382</v>
+        <v>2.803989064043998</v>
       </c>
     </row>
     <row r="33">
@@ -4042,10 +4042,10 @@
         <v>0.2250238576876559</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.9086893028484713</v>
+        <v>-0.9086893046163037</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.8995969692070245</v>
+        <v>-0.8995969717554908</v>
       </c>
       <c r="L33" t="n">
         <v>348.15</v>
@@ -4057,10 +4057,10 @@
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="n">
-        <v>6.796093401777417</v>
+        <v>6.796093411600431</v>
       </c>
       <c r="T33" t="n">
-        <v>0.4840475892286084</v>
+        <v>0.4840475893002401</v>
       </c>
       <c r="U33" t="n">
         <v>348.15</v>
@@ -4078,13 +4078,13 @@
         <v>3.273739172051632</v>
       </c>
       <c r="Z33" t="n">
-        <v>3.29596779874024</v>
+        <v>3.295967796827624</v>
       </c>
       <c r="AA33" t="n">
-        <v>0.7594852916714075</v>
+        <v>0.7594852917000162</v>
       </c>
       <c r="AB33" t="n">
-        <v>0.7612533676702381</v>
+        <v>0.7612533675464035</v>
       </c>
       <c r="AC33" t="inlineStr"/>
       <c r="AD33" t="inlineStr"/>
@@ -4123,10 +4123,10 @@
         <v>0.3037556803052021</v>
       </c>
       <c r="J34" t="n">
-        <v>-1.080153912870865</v>
+        <v>-1.080153914605717</v>
       </c>
       <c r="K34" t="n">
-        <v>-1.073731368406063</v>
+        <v>-1.073731371015842</v>
       </c>
       <c r="L34" t="n">
         <v>348.15</v>
@@ -4138,10 +4138,10 @@
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="n">
-        <v>6.796093401777642</v>
+        <v>6.796093411600406</v>
       </c>
       <c r="T34" t="n">
-        <v>0.5773541496893602</v>
+        <v>0.5773541498247756</v>
       </c>
       <c r="U34" t="n">
         <v>348.15</v>
@@ -4159,13 +4159,13 @@
         <v>2.753124566956449</v>
       </c>
       <c r="Z34" t="n">
-        <v>2.76736887802441</v>
+        <v>2.767368876080485</v>
       </c>
       <c r="AA34" t="n">
-        <v>0.6917170570515829</v>
+        <v>0.6917170571004315</v>
       </c>
       <c r="AB34" t="n">
-        <v>0.6925905627791673</v>
+        <v>0.6925905627086169</v>
       </c>
       <c r="AC34" t="inlineStr"/>
       <c r="AD34" t="inlineStr"/>
@@ -4204,10 +4204,10 @@
         <v>0.404700941454108</v>
       </c>
       <c r="J35" t="n">
-        <v>-1.236894617544212</v>
+        <v>-1.236894619207107</v>
       </c>
       <c r="K35" t="n">
-        <v>-1.230507619639397</v>
+        <v>-1.230507621951563</v>
       </c>
       <c r="L35" t="n">
         <v>348.15</v>
@@ -4219,10 +4219,10 @@
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="n">
-        <v>6.796093401777705</v>
+        <v>6.796093411600405</v>
       </c>
       <c r="T35" t="n">
-        <v>0.7565591496835401</v>
+        <v>0.7565591499614169</v>
       </c>
       <c r="U35" t="n">
         <v>348.15</v>
@@ -4240,13 +4240,13 @@
         <v>2.273800640382512</v>
       </c>
       <c r="Z35" t="n">
-        <v>2.286508035978668</v>
+        <v>2.286508034684095</v>
       </c>
       <c r="AA35" t="n">
-        <v>0.6337571208873647</v>
+        <v>0.6337571209777125</v>
       </c>
       <c r="AB35" t="n">
-        <v>0.6342731723041383</v>
+        <v>0.6342731723418636</v>
       </c>
       <c r="AC35" t="inlineStr"/>
       <c r="AD35" t="inlineStr"/>
@@ -4285,10 +4285,10 @@
         <v>0.5369373382100668</v>
       </c>
       <c r="J36" t="n">
-        <v>-1.347018323521022</v>
+        <v>-1.347018324998745</v>
       </c>
       <c r="K36" t="n">
-        <v>-1.336991914986568</v>
+        <v>-1.336991916552356</v>
       </c>
       <c r="L36" t="n">
         <v>348.15</v>
@@ -4300,10 +4300,10 @@
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="n">
-        <v>6.796093401777652</v>
+        <v>6.796093411600436</v>
       </c>
       <c r="T36" t="n">
-        <v>1.148166112876005</v>
+        <v>1.148166113532917</v>
       </c>
       <c r="U36" t="n">
         <v>348.15</v>
@@ -4321,13 +4321,13 @@
         <v>1.840123941197469</v>
       </c>
       <c r="Z36" t="n">
-        <v>1.857699457999926</v>
+        <v>1.857699457844061</v>
       </c>
       <c r="AA36" t="n">
-        <v>0.5978100749597839</v>
+        <v>0.5978100751557112</v>
       </c>
       <c r="AB36" t="n">
-        <v>0.598121284380675</v>
+        <v>0.5981212845742052</v>
       </c>
       <c r="AC36" t="inlineStr"/>
       <c r="AD36" t="inlineStr"/>
@@ -4366,10 +4366,10 @@
         <v>0.7233840860253505</v>
       </c>
       <c r="J37" t="n">
-        <v>-1.242210688860153</v>
+        <v>-1.242210689684903</v>
       </c>
       <c r="K37" t="n">
-        <v>-1.240674530803729</v>
+        <v>-1.240674531245923</v>
       </c>
       <c r="L37" t="n">
         <v>348.15</v>
@@ -4381,10 +4381,10 @@
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="n">
-        <v>6.796093401777383</v>
+        <v>6.79609341160043</v>
       </c>
       <c r="T37" t="n">
-        <v>2.260981924010916</v>
+        <v>2.260981926056945</v>
       </c>
       <c r="U37" t="n">
         <v>348.15</v>
@@ -4402,13 +4402,13 @@
         <v>1.481823228383789</v>
       </c>
       <c r="Z37" t="n">
-        <v>1.484086429160632</v>
+        <v>1.484086429724217</v>
       </c>
       <c r="AA37" t="n">
-        <v>0.6580001755551571</v>
+        <v>0.6580001762005196</v>
       </c>
       <c r="AB37" t="n">
-        <v>0.6580067642779811</v>
+        <v>0.6580067649251968</v>
       </c>
       <c r="AC37" t="inlineStr"/>
       <c r="AD37" t="inlineStr"/>
@@ -4447,10 +4447,10 @@
         <v>0.8462269658613781</v>
       </c>
       <c r="J38" t="n">
-        <v>-0.9178544645297882</v>
+        <v>-0.9178544643803006</v>
       </c>
       <c r="K38" t="n">
-        <v>-0.9142149665461294</v>
+        <v>-0.9142149665302396</v>
       </c>
       <c r="L38" t="n">
         <v>348.15</v>
@@ -4462,10 +4462,10 @@
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="n">
-        <v>6.796093401777684</v>
+        <v>6.796093411600427</v>
       </c>
       <c r="T38" t="n">
-        <v>3.661933525411112</v>
+        <v>3.661933529591923</v>
       </c>
       <c r="U38" t="n">
         <v>348.15</v>
@@ -4483,13 +4483,13 @@
         <v>1.327553460577857</v>
       </c>
       <c r="Z38" t="n">
-        <v>1.332147067461135</v>
+        <v>1.33214706729013</v>
       </c>
       <c r="AA38" t="n">
-        <v>0.8756495625491686</v>
+        <v>0.8756495642609963</v>
       </c>
       <c r="AB38" t="n">
-        <v>0.8758117982712791</v>
+        <v>0.8758117999788461</v>
       </c>
       <c r="AC38" t="inlineStr"/>
       <c r="AD38" t="inlineStr"/>
@@ -4528,7 +4528,7 @@
         <v>1</v>
       </c>
       <c r="J39" t="n">
-        <v>0.004862123427372522</v>
+        <v>0.004862126082543827</v>
       </c>
       <c r="K39" t="n">
         <v>-0</v>
@@ -4543,10 +4543,10 @@
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="n">
-        <v>6.796093401777657</v>
+        <v>6.796093411600445</v>
       </c>
       <c r="T39" t="n">
-        <v>6.796093401777661</v>
+        <v>6.796093411600459</v>
       </c>
       <c r="U39" t="n">
         <v>348.15</v>
@@ -4564,13 +4564,13 @@
         <v>1.183643303079099</v>
       </c>
       <c r="Z39" t="n">
-        <v>1.179170144599812</v>
+        <v>1.179170142167497</v>
       </c>
       <c r="AA39" t="n">
-        <v>2.051843765579041</v>
+        <v>2.051843774731533</v>
       </c>
       <c r="AB39" t="n">
-        <v>2.049637537108848</v>
+        <v>2.049637545037226</v>
       </c>
       <c r="AC39" t="inlineStr"/>
       <c r="AD39" t="inlineStr"/>
@@ -4609,7 +4609,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>0.006870537577241487</v>
+        <v>0.006870536186267373</v>
       </c>
       <c r="K40" t="n">
         <v>-0</v>
@@ -4624,7 +4624,7 @@
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="n">
-        <v>7.321032612720305</v>
+        <v>7.321032623375861</v>
       </c>
       <c r="T40" t="n">
         <v>0.3856235728691537</v>
@@ -4645,13 +4645,13 @@
         <v>6.61461467890805</v>
       </c>
       <c r="Z40" t="n">
-        <v>6.589328014701029</v>
+        <v>6.589328019813424</v>
       </c>
       <c r="AA40" t="n">
         <v>1.319198569296742</v>
       </c>
       <c r="AB40" t="n">
-        <v>1.315193816278755</v>
+        <v>1.31519381708775</v>
       </c>
       <c r="AC40" t="inlineStr"/>
       <c r="AD40" t="inlineStr"/>
@@ -4690,10 +4690,10 @@
         <v>0.0313429431018967</v>
       </c>
       <c r="J41" t="n">
-        <v>-0.1733331826404315</v>
+        <v>-0.1733331840288128</v>
       </c>
       <c r="K41" t="n">
-        <v>-0.17733687540671</v>
+        <v>-0.1773368762476727</v>
       </c>
       <c r="L41" t="n">
         <v>363.15</v>
@@ -4705,10 +4705,10 @@
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="n">
-        <v>7.321032612720032</v>
+        <v>7.321032623375828</v>
       </c>
       <c r="T41" t="n">
-        <v>0.395529438171021</v>
+        <v>0.3955294381759807</v>
       </c>
       <c r="U41" t="n">
         <v>363.15</v>
@@ -4726,13 +4726,13 @@
         <v>5.896826143419265</v>
       </c>
       <c r="Z41" t="n">
-        <v>5.883178331233971</v>
+        <v>5.883178333098549</v>
       </c>
       <c r="AA41" t="n">
-        <v>1.1916705596849</v>
+        <v>1.191670559687992</v>
       </c>
       <c r="AB41" t="n">
-        <v>1.189662392777172</v>
+        <v>1.18966239305446</v>
       </c>
       <c r="AC41" t="inlineStr"/>
       <c r="AD41" t="inlineStr"/>
@@ -4771,10 +4771,10 @@
         <v>0.06769199592074771</v>
       </c>
       <c r="J42" t="n">
-        <v>-0.3469912832382113</v>
+        <v>-0.3469912846224715</v>
       </c>
       <c r="K42" t="n">
-        <v>-0.3597698528586217</v>
+        <v>-0.3597698544620648</v>
       </c>
       <c r="L42" t="n">
         <v>363.15</v>
@@ -4786,10 +4786,10 @@
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="n">
-        <v>7.321032612720104</v>
+        <v>7.321032623375882</v>
       </c>
       <c r="T42" t="n">
-        <v>0.4106970499914484</v>
+        <v>0.4106970500042402</v>
       </c>
       <c r="U42" t="n">
         <v>363.15</v>
@@ -4807,13 +4807,13 @@
         <v>5.244535733644222</v>
       </c>
       <c r="Z42" t="n">
-        <v>5.204161022304977</v>
+        <v>5.204161021614214</v>
       </c>
       <c r="AA42" t="n">
-        <v>1.079816205312328</v>
+        <v>1.079816205319582</v>
       </c>
       <c r="AB42" t="n">
-        <v>1.074376456669699</v>
+        <v>1.074376456584041</v>
       </c>
       <c r="AC42" t="inlineStr"/>
       <c r="AD42" t="inlineStr"/>
@@ -4852,10 +4852,10 @@
         <v>0.1107704362966803</v>
       </c>
       <c r="J43" t="n">
-        <v>-0.5445608039508207</v>
+        <v>-0.5445608053284651</v>
       </c>
       <c r="K43" t="n">
-        <v>-0.547623426805799</v>
+        <v>-0.5476234290551744</v>
       </c>
       <c r="L43" t="n">
         <v>363.15</v>
@@ -4867,10 +4867,10 @@
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="n">
-        <v>7.321032612718562</v>
+        <v>7.321032623375856</v>
       </c>
       <c r="T43" t="n">
-        <v>0.4341615021107803</v>
+        <v>0.4341615021362346</v>
       </c>
       <c r="U43" t="n">
         <v>363.15</v>
@@ -4888,13 +4888,13 @@
         <v>4.559383201093018</v>
       </c>
       <c r="Z43" t="n">
-        <v>4.550477740524381</v>
+        <v>4.550477737991204</v>
       </c>
       <c r="AA43" t="n">
-        <v>0.9697523385370898</v>
+        <v>0.9697523385500958</v>
       </c>
       <c r="AB43" t="n">
-        <v>0.9686788841666892</v>
+        <v>0.9686788838745022</v>
       </c>
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" t="inlineStr"/>
@@ -4933,10 +4933,10 @@
         <v>0.1621830135089458</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.7265419994421152</v>
+        <v>-0.7265420008084362</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.7374233648997633</v>
+        <v>-0.7374233676138454</v>
       </c>
       <c r="L44" t="n">
         <v>363.15</v>
@@ -4948,10 +4948,10 @@
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="n">
-        <v>7.321032612722156</v>
+        <v>7.321032623375888</v>
       </c>
       <c r="T44" t="n">
-        <v>0.4708399064487639</v>
+        <v>0.4708399064952365</v>
       </c>
       <c r="U44" t="n">
         <v>363.15</v>
@@ -4969,13 +4969,13 @@
         <v>3.961588104581543</v>
       </c>
       <c r="Z44" t="n">
-        <v>3.932483402602049</v>
+        <v>3.932483399005681</v>
       </c>
       <c r="AA44" t="n">
-        <v>0.8765606954399744</v>
+        <v>0.8765606954614614</v>
       </c>
       <c r="AB44" t="n">
-        <v>0.8734914928698186</v>
+        <v>0.8734914925128116</v>
       </c>
       <c r="AC44" t="inlineStr"/>
       <c r="AD44" t="inlineStr"/>
@@ -5014,10 +5014,10 @@
         <v>0.2248843778792036</v>
       </c>
       <c r="J45" t="n">
-        <v>-0.9223512873985555</v>
+        <v>-0.9223512887455074</v>
       </c>
       <c r="K45" t="n">
-        <v>-0.9270023758423882</v>
+        <v>-0.9270023787686474</v>
       </c>
       <c r="L45" t="n">
         <v>363.15</v>
@@ -5029,10 +5029,10 @@
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="n">
-        <v>7.32103261272012</v>
+        <v>7.321032623375917</v>
       </c>
       <c r="T45" t="n">
-        <v>0.5305123641898326</v>
+        <v>0.5305123642735075</v>
       </c>
       <c r="U45" t="n">
         <v>363.15</v>
@@ -5050,13 +5050,13 @@
         <v>3.363989721784967</v>
       </c>
       <c r="Z45" t="n">
-        <v>3.352646522207342</v>
+        <v>3.352646518359964</v>
       </c>
       <c r="AA45" t="n">
-        <v>0.7892099518827772</v>
+        <v>0.7892099519175315</v>
       </c>
       <c r="AB45" t="n">
-        <v>0.7882055676595546</v>
+        <v>0.7882055673539666</v>
       </c>
       <c r="AC45" t="inlineStr"/>
       <c r="AD45" t="inlineStr"/>
@@ -5095,10 +5095,10 @@
         <v>0.303315168283936</v>
       </c>
       <c r="J46" t="n">
-        <v>-1.108033339296409</v>
+        <v>-1.108033340605969</v>
       </c>
       <c r="K46" t="n">
-        <v>-1.112233521495927</v>
+        <v>-1.11223352430042</v>
       </c>
       <c r="L46" t="n">
         <v>363.15</v>
@@ -5110,10 +5110,10 @@
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="n">
-        <v>7.321032612720164</v>
+        <v>7.32103262337585</v>
       </c>
       <c r="T46" t="n">
-        <v>0.6340262764512471</v>
+        <v>0.6340262766071267</v>
       </c>
       <c r="U46" t="n">
         <v>363.15</v>
@@ -5131,13 +5131,13 @@
         <v>2.822546096363733</v>
       </c>
       <c r="Z46" t="n">
-        <v>2.813267363001214</v>
+        <v>2.813267359702474</v>
       </c>
       <c r="AA46" t="n">
-        <v>0.7133156374301105</v>
+        <v>0.7133156374881875</v>
       </c>
       <c r="AB46" t="n">
-        <v>0.7126686629154462</v>
+        <v>0.712668662743731</v>
       </c>
       <c r="AC46" t="inlineStr"/>
       <c r="AD46" t="inlineStr"/>
@@ -5176,10 +5176,10 @@
         <v>0.4035535783740583</v>
       </c>
       <c r="J47" t="n">
-        <v>-1.279027371824528</v>
+        <v>-1.279027373053689</v>
       </c>
       <c r="K47" t="n">
-        <v>-1.281836479723555</v>
+        <v>-1.281836482019501</v>
       </c>
       <c r="L47" t="n">
         <v>363.15</v>
@@ -5191,10 +5191,10 @@
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="n">
-        <v>7.321032612720308</v>
+        <v>7.321032623375931</v>
       </c>
       <c r="T47" t="n">
-        <v>0.8300906431101825</v>
+        <v>0.8300906434248547</v>
       </c>
       <c r="U47" t="n">
         <v>363.15</v>
@@ -5212,13 +5212,13 @@
         <v>2.32444162889002</v>
       </c>
       <c r="Z47" t="n">
-        <v>2.318881081965389</v>
+        <v>2.318881079855415</v>
       </c>
       <c r="AA47" t="n">
-        <v>0.6499504109583785</v>
+        <v>0.6499504110635456</v>
       </c>
       <c r="AB47" t="n">
-        <v>0.6496813470170616</v>
+        <v>0.6496813470201801</v>
       </c>
       <c r="AC47" t="inlineStr"/>
       <c r="AD47" t="inlineStr"/>
@@ -5257,10 +5257,10 @@
         <v>0.5374034102962609</v>
       </c>
       <c r="J48" t="n">
-        <v>-1.394309602744418</v>
+        <v>-1.39430960376377</v>
       </c>
       <c r="K48" t="n">
-        <v>-1.401953085018864</v>
+        <v>-1.401953086481821</v>
       </c>
       <c r="L48" t="n">
         <v>363.15</v>
@@ -5272,10 +5272,10 @@
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="n">
-        <v>7.321032612720578</v>
+        <v>7.321032623375884</v>
       </c>
       <c r="T48" t="n">
-        <v>1.264260317920422</v>
+        <v>1.264260318662645</v>
       </c>
       <c r="U48" t="n">
         <v>363.15</v>
@@ -5293,13 +5293,13 @@
         <v>1.880086809874968</v>
       </c>
       <c r="Z48" t="n">
-        <v>1.866783656015905</v>
+        <v>1.86678365524679</v>
       </c>
       <c r="AA48" t="n">
-        <v>0.613156963306853</v>
+        <v>0.6131569635346641</v>
       </c>
       <c r="AB48" t="n">
-        <v>0.6128244032109624</v>
+        <v>0.6128244034192779</v>
       </c>
       <c r="AC48" t="inlineStr"/>
       <c r="AD48" t="inlineStr"/>
@@ -5338,10 +5338,10 @@
         <v>0.7231615990865421</v>
       </c>
       <c r="J49" t="n">
-        <v>-1.281847224891087</v>
+        <v>-1.28184722519189</v>
       </c>
       <c r="K49" t="n">
-        <v>-1.303809239719071</v>
+        <v>-1.30380924038677</v>
       </c>
       <c r="L49" t="n">
         <v>363.15</v>
@@ -5353,10 +5353,10 @@
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="n">
-        <v>7.321032612720116</v>
+        <v>7.321032623375888</v>
       </c>
       <c r="T49" t="n">
-        <v>2.468002614762002</v>
+        <v>2.468002617027278</v>
       </c>
       <c r="U49" t="n">
         <v>363.15</v>
@@ -5374,13 +5374,13 @@
         <v>1.510150050873902</v>
       </c>
       <c r="Z49" t="n">
-        <v>1.478258899653195</v>
+        <v>1.478258899133168</v>
       </c>
       <c r="AA49" t="n">
-        <v>0.6887420788538964</v>
+        <v>0.6887420796047706</v>
       </c>
       <c r="AB49" t="n">
-        <v>0.6883165857224972</v>
+        <v>0.6883165864625062</v>
       </c>
       <c r="AC49" t="inlineStr"/>
       <c r="AD49" t="inlineStr"/>
@@ -5419,10 +5419,10 @@
         <v>0.8465004587575707</v>
       </c>
       <c r="J50" t="n">
-        <v>-0.9709560742595975</v>
+        <v>-0.9709560735119499</v>
       </c>
       <c r="K50" t="n">
-        <v>-0.9580743526900469</v>
+        <v>-0.9580743531138255</v>
       </c>
       <c r="L50" t="n">
         <v>363.15</v>
@@ -5434,10 +5434,10 @@
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="inlineStr"/>
       <c r="S50" t="n">
-        <v>7.321032612720071</v>
+        <v>7.321032623375924</v>
       </c>
       <c r="T50" t="n">
-        <v>3.981296002805732</v>
+        <v>3.981296007401405</v>
       </c>
       <c r="U50" t="n">
         <v>363.15</v>
@@ -5455,13 +5455,13 @@
         <v>1.301760158887947</v>
       </c>
       <c r="Z50" t="n">
-        <v>1.317277897656628</v>
+        <v>1.317277896228169</v>
       </c>
       <c r="AA50" t="n">
-        <v>0.9450888485648006</v>
+        <v>0.9450888505860603</v>
       </c>
       <c r="AB50" t="n">
-        <v>0.9460643246844582</v>
+        <v>0.9460643266254739</v>
       </c>
       <c r="AC50" t="inlineStr"/>
       <c r="AD50" t="inlineStr"/>
@@ -5500,7 +5500,7 @@
         <v>1</v>
       </c>
       <c r="J51" t="n">
-        <v>-0.002874066992278601</v>
+        <v>-0.002874063579671265</v>
       </c>
       <c r="K51" t="n">
         <v>-0</v>
@@ -5515,10 +5515,10 @@
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="n">
-        <v>7.321032612720397</v>
+        <v>7.32103262337589</v>
       </c>
       <c r="T51" t="n">
-        <v>7.321032612720393</v>
+        <v>7.321032623375888</v>
       </c>
       <c r="U51" t="n">
         <v>363.15</v>
@@ -5536,13 +5536,13 @@
         <v>1.152400980781263</v>
       </c>
       <c r="Z51" t="n">
-        <v>1.154863361315</v>
+        <v>1.154863358384558</v>
       </c>
       <c r="AA51" t="n">
-        <v>2.352652164760153</v>
+        <v>2.352652176061142</v>
       </c>
       <c r="AB51" t="n">
-        <v>2.354392846903258</v>
+        <v>2.354392856152213</v>
       </c>
       <c r="AC51" t="inlineStr"/>
       <c r="AD51" t="inlineStr"/>
@@ -5581,7 +5581,7 @@
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>-0.003616187205238874</v>
+        <v>-0.003616187462445686</v>
       </c>
       <c r="K52" t="n">
         <v>-0</v>
@@ -5596,7 +5596,7 @@
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="n">
-        <v>8.061020980589207</v>
+        <v>8.061020990332429</v>
       </c>
       <c r="T52" t="n">
         <v>0.4223077491365858</v>
@@ -5617,13 +5617,13 @@
         <v>6.700456301074103</v>
       </c>
       <c r="Z52" t="n">
-        <v>6.714214586332216</v>
+        <v>6.714214587311663</v>
       </c>
       <c r="AA52" t="n">
         <v>1.396069497179098</v>
       </c>
       <c r="AB52" t="n">
-        <v>1.398255996140206</v>
+        <v>1.398255996295874</v>
       </c>
       <c r="AC52" t="inlineStr"/>
       <c r="AD52" t="inlineStr"/>
@@ -5662,10 +5662,10 @@
         <v>0.01510867499299501</v>
       </c>
       <c r="J53" t="n">
-        <v>-0.08424000352235422</v>
+        <v>-0.08424000377832552</v>
       </c>
       <c r="K53" t="n">
-        <v>-0.08958067421777703</v>
+        <v>-0.08958067479466918</v>
       </c>
       <c r="L53" t="n">
         <v>383.15</v>
@@ -5677,10 +5677,10 @@
       <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr"/>
       <c r="S53" t="n">
-        <v>8.061020980589035</v>
+        <v>8.061020990332281</v>
       </c>
       <c r="T53" t="n">
-        <v>0.4280471220763823</v>
+        <v>0.4280471220787501</v>
       </c>
       <c r="U53" t="n">
         <v>383.15</v>
@@ -5698,13 +5698,13 @@
         <v>6.367204815680409</v>
       </c>
       <c r="Z53" t="n">
-        <v>6.347754119248409</v>
+        <v>6.347754118081134</v>
       </c>
       <c r="AA53" t="n">
-        <v>1.33302751981244</v>
+        <v>1.333027519814086</v>
       </c>
       <c r="AB53" t="n">
-        <v>1.329990140869432</v>
+        <v>1.329990140688839</v>
       </c>
       <c r="AC53" t="inlineStr"/>
       <c r="AD53" t="inlineStr"/>

</xml_diff>